<commit_message>
Auslagern von Excel_Auswertung als eigenes Programm
kwt
</commit_message>
<xml_diff>
--- a/Daten_Vergleich.xlsx
+++ b/Daten_Vergleich.xlsx
@@ -394,10 +394,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.001538461538461538</v>
+        <v>0.27</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -408,16 +408,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="B3">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>0.305</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1.222222222222222</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -425,16 +425,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4">
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>0.38</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1.105263157894737</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -442,1056 +442,1056 @@
     </row>
     <row r="5" spans="1:6">
       <c r="B5">
-        <v>0</v>
+        <v>2.588235294117647</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>0.425</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1.051546391752577</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="F5">
-        <v>0</v>
+        <v>0.005</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6">
-        <v>0</v>
+        <v>2.227272727272727</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1.041322314049587</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F6">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7">
-        <v>0</v>
+        <v>2.4375</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>0.58</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1.034965034965035</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>0.135</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>0.025</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8">
-        <v>0</v>
+        <v>2.384615384615385</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>0.605</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1.032258064516129</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>0.16</v>
       </c>
       <c r="F8">
-        <v>0</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="B9">
-        <v>0</v>
+        <v>2.511111111111111</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>0.625</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1.03030303030303</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>0.19</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>0.035</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10">
-        <v>0</v>
+        <v>2.527272727272727</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1.022857142857143</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>0.235</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11">
-        <v>0</v>
+        <v>2.421875</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.59</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1.02247191011236</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>0.28</v>
       </c>
       <c r="F11">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12">
-        <v>0</v>
+        <v>2.397260273972603</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.5649999999999999</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1.021978021978022</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>0.325</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13">
-        <v>0</v>
+        <v>2.25</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>0.545</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1.016129032258065</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14">
-        <v>0</v>
+        <v>2.467391304347826</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1.01063829787234</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="F14">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15">
-        <v>0</v>
+        <v>2.673267326732673</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>0.465</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1.010416666666667</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>0.465</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16">
-        <v>0</v>
+        <v>2.663716814159292</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>0.405</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1.010416666666667</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>0.52</v>
       </c>
       <c r="F16">
-        <v>0</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17">
-        <v>0</v>
+        <v>2.758064516129032</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>0.35</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1.010416666666667</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>0.575</v>
       </c>
       <c r="F17">
-        <v>0</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18">
-        <v>0</v>
+        <v>2.772727272727273</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1.010309278350515</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>0.615</v>
       </c>
       <c r="F18">
-        <v>0</v>
+        <v>0.045</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19">
-        <v>0</v>
+        <v>2.685714285714285</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.29</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1.010204081632653</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>0.65</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20">
-        <v>0</v>
+        <v>2.701388888888889</v>
       </c>
       <c r="C20">
-        <v>0</v>
+        <v>0.27</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1.010204081632653</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21">
-        <v>0</v>
+        <v>2.662251655629139</v>
       </c>
       <c r="C21">
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1.005102040816326</v>
       </c>
       <c r="E21">
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22">
-        <v>0</v>
+        <v>2.651315789473684</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>0.235</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>1.005050505050505</v>
       </c>
       <c r="E22">
-        <v>0</v>
+        <v>0.705</v>
       </c>
       <c r="F22">
-        <v>0</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23">
-        <v>0</v>
+        <v>2.621794871794872</v>
       </c>
       <c r="C23">
-        <v>0</v>
+        <v>0.215</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1.005050505050505</v>
       </c>
       <c r="E23">
-        <v>0</v>
+        <v>0.725</v>
       </c>
       <c r="F23">
-        <v>0</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24">
-        <v>0</v>
+        <v>2.611111111111111</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>0.185</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1.005050505050505</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>0.755</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25">
-        <v>0</v>
+        <v>2.6</v>
       </c>
       <c r="C25">
-        <v>0</v>
+        <v>0.175</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1.005025125628141</v>
       </c>
       <c r="E25">
-        <v>0</v>
+        <v>0.77</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26">
-        <v>0</v>
+        <v>2.590361445783132</v>
       </c>
       <c r="C26">
-        <v>0</v>
+        <v>0.17</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1.005025125628141</v>
       </c>
       <c r="E26">
-        <v>0</v>
+        <v>0.775</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>0.055</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27">
-        <v>0</v>
+        <v>2.558823529411764</v>
       </c>
       <c r="C27">
-        <v>0</v>
+        <v>0.155</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1.005</v>
       </c>
       <c r="E27">
-        <v>0</v>
+        <v>0.79</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28">
-        <v>0</v>
+        <v>2.558823529411764</v>
       </c>
       <c r="C28">
-        <v>0</v>
+        <v>0.155</v>
       </c>
       <c r="D28">
-        <v>0</v>
+        <v>1.005</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>0.79</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29">
-        <v>0</v>
+        <v>2.540229885057471</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>0.135</v>
       </c>
       <c r="D29">
-        <v>0</v>
+        <v>1.005</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>0.805</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30">
-        <v>0</v>
+        <v>2.51685393258427</v>
       </c>
       <c r="C30">
-        <v>0</v>
+        <v>0.115</v>
       </c>
       <c r="D30">
-        <v>0</v>
+        <v>1.005</v>
       </c>
       <c r="E30">
-        <v>0</v>
+        <v>0.825</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31">
-        <v>0</v>
+        <v>2.540983606557377</v>
       </c>
       <c r="C31">
-        <v>0</v>
+        <v>0.08500000000000001</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31">
-        <v>0</v>
+        <v>0.85</v>
       </c>
       <c r="F31">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32">
-        <v>0</v>
+        <v>2.527173913043478</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>0.855</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33">
-        <v>0</v>
+        <v>2.505376344086022</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>0.865</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34">
-        <v>0</v>
+        <v>2.505376344086022</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>0.865</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="35" spans="2:6">
       <c r="B35">
-        <v>0</v>
+        <v>2.505376344086022</v>
       </c>
       <c r="C35">
-        <v>0</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>0.865</v>
       </c>
       <c r="F35">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="36" spans="2:6">
       <c r="B36">
-        <v>0</v>
+        <v>2.505376344086022</v>
       </c>
       <c r="C36">
-        <v>0</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>0.865</v>
       </c>
       <c r="F36">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="37" spans="2:6">
       <c r="B37">
-        <v>0</v>
+        <v>2.492063492063492</v>
       </c>
       <c r="C37">
-        <v>0</v>
+        <v>0.055</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="F37">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="38" spans="2:6">
       <c r="B38">
-        <v>0</v>
+        <v>2.492063492063492</v>
       </c>
       <c r="C38">
-        <v>0</v>
+        <v>0.055</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="F38">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="39" spans="2:6">
       <c r="B39">
-        <v>0</v>
+        <v>2.492063492063492</v>
       </c>
       <c r="C39">
-        <v>0</v>
+        <v>0.055</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39">
-        <v>0</v>
+        <v>0.88</v>
       </c>
       <c r="F39">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="40" spans="2:6">
       <c r="B40">
-        <v>0</v>
+        <v>2.489473684210526</v>
       </c>
       <c r="C40">
-        <v>0</v>
+        <v>0.05</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>0.885</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="41" spans="2:6">
       <c r="B41">
-        <v>0</v>
+        <v>2.505208333333333</v>
       </c>
       <c r="C41">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>0.895</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="42" spans="2:6">
       <c r="B42">
-        <v>0</v>
+        <v>2.556701030927835</v>
       </c>
       <c r="C42">
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E42">
-        <v>0</v>
+        <v>0.905</v>
       </c>
       <c r="F42">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="43" spans="2:6">
       <c r="B43">
-        <v>0</v>
+        <v>2.548717948717949</v>
       </c>
       <c r="C43">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E43">
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="F43">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="44" spans="2:6">
       <c r="B44">
-        <v>0</v>
+        <v>2.548717948717949</v>
       </c>
       <c r="C44">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E44">
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="F44">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="45" spans="2:6">
       <c r="B45">
-        <v>0</v>
+        <v>2.548717948717949</v>
       </c>
       <c r="C45">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="F45">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="46" spans="2:6">
       <c r="B46">
-        <v>0</v>
+        <v>2.548717948717949</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>0.91</v>
       </c>
       <c r="F46">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="47" spans="2:6">
       <c r="B47">
-        <v>0</v>
+        <v>2.535714285714286</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47">
-        <v>0</v>
+        <v>0.915</v>
       </c>
       <c r="F47">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="48" spans="2:6">
       <c r="B48">
-        <v>0</v>
+        <v>2.535714285714286</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48">
-        <v>0</v>
+        <v>0.915</v>
       </c>
       <c r="F48">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="49" spans="2:6">
       <c r="B49">
-        <v>0</v>
+        <v>2.535714285714286</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>0.915</v>
       </c>
       <c r="F49">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="50" spans="2:6">
       <c r="B50">
-        <v>0</v>
+        <v>2.515151515151515</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E50">
-        <v>0</v>
+        <v>0.925</v>
       </c>
       <c r="F50">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="51" spans="2:6">
       <c r="B51">
-        <v>0</v>
+        <v>2.515151515151515</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51">
-        <v>0</v>
+        <v>0.925</v>
       </c>
       <c r="F51">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="52" spans="2:6">
       <c r="B52">
-        <v>0</v>
+        <v>2.515151515151515</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E52">
-        <v>0</v>
+        <v>0.925</v>
       </c>
       <c r="F52">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="53" spans="2:6">
       <c r="B53">
-        <v>0</v>
+        <v>2.515151515151515</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E53">
-        <v>0</v>
+        <v>0.925</v>
       </c>
       <c r="F53">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="54" spans="2:6">
       <c r="B54">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E54">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F54">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="55" spans="2:6">
       <c r="B55">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C55">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F55">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="56" spans="2:6">
       <c r="B56">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C56">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F56">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="57" spans="2:6">
       <c r="B57">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C57">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E57">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="58" spans="2:6">
       <c r="B58">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C58">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E58">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="59" spans="2:6">
       <c r="B59">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E59">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F59">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="60" spans="2:6">
       <c r="B60">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E60">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F60">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="61" spans="2:6">
       <c r="B61">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F61">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="62" spans="2:6">
       <c r="B62">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E62">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F62">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="63" spans="2:6">
       <c r="B63">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C63">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E63">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="64" spans="2:6">
       <c r="B64">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C64">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E64">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="65" spans="2:6">
       <c r="B65">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E65">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F65">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="66" spans="2:6">
       <c r="B66">
-        <v>0</v>
+        <v>2.50251256281407</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>0.005</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>0.93</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>0.065</v>
       </c>
     </row>
     <row r="67" spans="2:6">

</xml_diff>

<commit_message>
Kleiner Bugfix Nachschub zum EXCEL Ding
kwt
</commit_message>
<xml_diff>
--- a/Daten_Vergleich.xlsx
+++ b/Daten_Vergleich.xlsx
@@ -394,10 +394,10 @@
         <v>0</v>
       </c>
       <c r="C2">
-        <v>0.27</v>
+        <v>0.01666666666666667</v>
       </c>
       <c r="D2">
-        <v>1.5</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -408,16 +408,16 @@
     </row>
     <row r="3" spans="1:6">
       <c r="B3">
-        <v>1.6</v>
+        <v>0</v>
       </c>
       <c r="C3">
-        <v>0.305</v>
+        <v>0.01666666666666667</v>
       </c>
       <c r="D3">
-        <v>1.222222222222222</v>
+        <v>1.2</v>
       </c>
       <c r="E3">
-        <v>0.025</v>
+        <v>0.003333333333333334</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -425,16 +425,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="C4">
-        <v>0.38</v>
+        <v>0.02333333333333333</v>
       </c>
       <c r="D4">
-        <v>1.105263157894737</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="E4">
-        <v>0.04</v>
+        <v>0.003333333333333334</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -442,911 +442,911 @@
     </row>
     <row r="5" spans="1:6">
       <c r="B5">
-        <v>2.588235294117647</v>
+        <v>0</v>
       </c>
       <c r="C5">
-        <v>0.425</v>
+        <v>0.03</v>
       </c>
       <c r="D5">
-        <v>1.051546391752577</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>0.08</v>
+        <v>0.003333333333333334</v>
       </c>
       <c r="F5">
-        <v>0.005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6">
-        <v>2.227272727272727</v>
+        <v>0</v>
       </c>
       <c r="C6">
-        <v>0.52</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="D6">
-        <v>1.041322314049587</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>0.1</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="F6">
-        <v>0.01</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="B7">
-        <v>2.4375</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <v>0.58</v>
+        <v>0.05666666666666666</v>
       </c>
       <c r="D7">
-        <v>1.034965034965035</v>
+        <v>1</v>
       </c>
       <c r="E7">
-        <v>0.135</v>
+        <v>0.006666666666666667</v>
       </c>
       <c r="F7">
-        <v>0.025</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="B8">
-        <v>2.384615384615385</v>
+        <v>0</v>
       </c>
       <c r="C8">
-        <v>0.605</v>
+        <v>0.07333333333333333</v>
       </c>
       <c r="D8">
-        <v>1.032258064516129</v>
+        <v>1</v>
       </c>
       <c r="E8">
-        <v>0.16</v>
+        <v>0.01</v>
       </c>
       <c r="F8">
-        <v>0.035</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="B9">
-        <v>2.511111111111111</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>0.625</v>
+        <v>0.1033333333333333</v>
       </c>
       <c r="D9">
-        <v>1.03030303030303</v>
+        <v>1</v>
       </c>
       <c r="E9">
-        <v>0.19</v>
+        <v>0.01</v>
       </c>
       <c r="F9">
-        <v>0.035</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10">
-        <v>2.527272727272727</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>0.62</v>
+        <v>0.1366666666666667</v>
       </c>
       <c r="D10">
-        <v>1.022857142857143</v>
+        <v>1</v>
       </c>
       <c r="E10">
-        <v>0.235</v>
+        <v>0.01</v>
       </c>
       <c r="F10">
-        <v>0.04</v>
+        <v>0.003333333333333334</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11">
-        <v>2.421875</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C11">
-        <v>0.59</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="D11">
-        <v>1.02247191011236</v>
+        <v>1</v>
       </c>
       <c r="E11">
-        <v>0.28</v>
+        <v>0.01666666666666667</v>
       </c>
       <c r="F11">
-        <v>0.04</v>
+        <v>0.003333333333333334</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12">
-        <v>2.397260273972603</v>
+        <v>0.75</v>
       </c>
       <c r="C12">
-        <v>0.5649999999999999</v>
+        <v>0.2366666666666667</v>
       </c>
       <c r="D12">
-        <v>1.021978021978022</v>
+        <v>1</v>
       </c>
       <c r="E12">
-        <v>0.325</v>
+        <v>0.02333333333333333</v>
       </c>
       <c r="F12">
-        <v>0.04</v>
+        <v>0.003333333333333334</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13">
-        <v>2.25</v>
+        <v>1.153846153846154</v>
       </c>
       <c r="C13">
-        <v>0.545</v>
+        <v>0.2633333333333333</v>
       </c>
       <c r="D13">
-        <v>1.016129032258065</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>0.36</v>
+        <v>0.03666666666666667</v>
       </c>
       <c r="F13">
-        <v>0.04</v>
+        <v>0.006666666666666667</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14">
-        <v>2.467391304347826</v>
+        <v>1.142857142857143</v>
       </c>
       <c r="C14">
-        <v>0.49</v>
+        <v>0.3033333333333333</v>
       </c>
       <c r="D14">
-        <v>1.01063829787234</v>
+        <v>1</v>
       </c>
       <c r="E14">
-        <v>0.42</v>
+        <v>0.06</v>
       </c>
       <c r="F14">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15">
-        <v>2.673267326732673</v>
+        <v>1.269230769230769</v>
       </c>
       <c r="C15">
-        <v>0.465</v>
+        <v>0.3166666666666667</v>
       </c>
       <c r="D15">
-        <v>1.010416666666667</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0.465</v>
+        <v>0.07666666666666666</v>
       </c>
       <c r="F15">
-        <v>0.04</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16">
-        <v>2.663716814159292</v>
+        <v>1.25</v>
       </c>
       <c r="C16">
-        <v>0.405</v>
+        <v>0.3233333333333333</v>
       </c>
       <c r="D16">
-        <v>1.010416666666667</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>0.52</v>
+        <v>0.09666666666666666</v>
       </c>
       <c r="F16">
-        <v>0.045</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17">
-        <v>2.758064516129032</v>
+        <v>1.230769230769231</v>
       </c>
       <c r="C17">
-        <v>0.35</v>
+        <v>0.3533333333333333</v>
       </c>
       <c r="D17">
-        <v>1.010416666666667</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0.575</v>
+        <v>0.12</v>
       </c>
       <c r="F17">
-        <v>0.045</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18">
-        <v>2.772727272727273</v>
+        <v>1.18</v>
       </c>
       <c r="C18">
-        <v>0.32</v>
+        <v>0.37</v>
       </c>
       <c r="D18">
-        <v>1.010309278350515</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>0.615</v>
+        <v>0.1533333333333333</v>
       </c>
       <c r="F18">
-        <v>0.045</v>
+        <v>0.01333333333333333</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19">
-        <v>2.685714285714285</v>
+        <v>1.392857142857143</v>
       </c>
       <c r="C19">
-        <v>0.29</v>
+        <v>0.3833333333333334</v>
       </c>
       <c r="D19">
-        <v>1.010204081632653</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0.65</v>
+        <v>0.17</v>
       </c>
       <c r="F19">
-        <v>0.05</v>
+        <v>0.01666666666666667</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20">
-        <v>2.701388888888889</v>
+        <v>1.701492537313433</v>
       </c>
       <c r="C20">
-        <v>0.27</v>
+        <v>0.3766666666666666</v>
       </c>
       <c r="D20">
-        <v>1.010204081632653</v>
+        <v>1</v>
       </c>
       <c r="E20">
-        <v>0.67</v>
+        <v>0.2066666666666667</v>
       </c>
       <c r="F20">
-        <v>0.05</v>
+        <v>0.01666666666666667</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21">
-        <v>2.662251655629139</v>
+        <v>1.736842105263158</v>
       </c>
       <c r="C21">
-        <v>0.23</v>
+        <v>0.36</v>
       </c>
       <c r="D21">
-        <v>1.005102040816326</v>
+        <v>1</v>
       </c>
       <c r="E21">
-        <v>0.7</v>
+        <v>0.2366666666666667</v>
       </c>
       <c r="F21">
-        <v>0.055</v>
+        <v>0.01666666666666667</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22">
-        <v>2.651315789473684</v>
+        <v>1.963855421686747</v>
       </c>
       <c r="C22">
-        <v>0.235</v>
+        <v>0.3733333333333334</v>
       </c>
       <c r="D22">
-        <v>1.005050505050505</v>
+        <v>1</v>
       </c>
       <c r="E22">
-        <v>0.705</v>
+        <v>0.2566666666666667</v>
       </c>
       <c r="F22">
-        <v>0.055</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23">
-        <v>2.621794871794872</v>
+        <v>1.943820224719101</v>
       </c>
       <c r="C23">
-        <v>0.215</v>
+        <v>0.37</v>
       </c>
       <c r="D23">
-        <v>1.005050505050505</v>
+        <v>1</v>
       </c>
       <c r="E23">
-        <v>0.725</v>
+        <v>0.2766666666666667</v>
       </c>
       <c r="F23">
-        <v>0.055</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24">
-        <v>2.611111111111111</v>
+        <v>1.928571428571429</v>
       </c>
       <c r="C24">
-        <v>0.185</v>
+        <v>0.3866666666666667</v>
       </c>
       <c r="D24">
-        <v>1.005050505050505</v>
+        <v>1</v>
       </c>
       <c r="E24">
-        <v>0.755</v>
+        <v>0.3066666666666666</v>
       </c>
       <c r="F24">
-        <v>0.055</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25">
-        <v>2.6</v>
+        <v>1.888888888888889</v>
       </c>
       <c r="C25">
-        <v>0.175</v>
+        <v>0.3833333333333334</v>
       </c>
       <c r="D25">
-        <v>1.005025125628141</v>
+        <v>1</v>
       </c>
       <c r="E25">
-        <v>0.77</v>
+        <v>0.34</v>
       </c>
       <c r="F25">
-        <v>0.055</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26">
-        <v>2.590361445783132</v>
+        <v>1.905982905982906</v>
       </c>
       <c r="C26">
-        <v>0.17</v>
+        <v>0.3866666666666667</v>
       </c>
       <c r="D26">
-        <v>1.005025125628141</v>
+        <v>1</v>
       </c>
       <c r="E26">
-        <v>0.775</v>
+        <v>0.37</v>
       </c>
       <c r="F26">
-        <v>0.055</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27">
-        <v>2.558823529411764</v>
+        <v>1.811023622047244</v>
       </c>
       <c r="C27">
-        <v>0.155</v>
+        <v>0.3933333333333333</v>
       </c>
       <c r="D27">
-        <v>1.005</v>
+        <v>1</v>
       </c>
       <c r="E27">
-        <v>0.79</v>
+        <v>0.4033333333333333</v>
       </c>
       <c r="F27">
-        <v>0.06</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28">
-        <v>2.558823529411764</v>
+        <v>1.876811594202898</v>
       </c>
       <c r="C28">
-        <v>0.155</v>
+        <v>0.4066666666666667</v>
       </c>
       <c r="D28">
-        <v>1.005</v>
+        <v>1</v>
       </c>
       <c r="E28">
-        <v>0.79</v>
+        <v>0.4366666666666666</v>
       </c>
       <c r="F28">
-        <v>0.06</v>
+        <v>0.02333333333333333</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29">
-        <v>2.540229885057471</v>
+        <v>1.888888888888889</v>
       </c>
       <c r="C29">
-        <v>0.135</v>
+        <v>0.4066666666666667</v>
       </c>
       <c r="D29">
-        <v>1.005</v>
+        <v>1</v>
       </c>
       <c r="E29">
-        <v>0.805</v>
+        <v>0.4566666666666667</v>
       </c>
       <c r="F29">
-        <v>0.065</v>
+        <v>0.02333333333333333</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30">
-        <v>2.51685393258427</v>
+        <v>1.855263157894737</v>
       </c>
       <c r="C30">
-        <v>0.115</v>
+        <v>0.4</v>
       </c>
       <c r="D30">
-        <v>1.005</v>
+        <v>1</v>
       </c>
       <c r="E30">
-        <v>0.825</v>
+        <v>0.48</v>
       </c>
       <c r="F30">
-        <v>0.065</v>
+        <v>0.02666666666666667</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31">
-        <v>2.540983606557377</v>
+        <v>1.895705521472393</v>
       </c>
       <c r="C31">
-        <v>0.08500000000000001</v>
+        <v>0.3666666666666666</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>0.85</v>
+        <v>0.5166666666666667</v>
       </c>
       <c r="F31">
-        <v>0.065</v>
+        <v>0.02666666666666667</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32">
-        <v>2.527173913043478</v>
+        <v>1.861271676300578</v>
       </c>
       <c r="C32">
-        <v>0.08</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>0.855</v>
+        <v>0.55</v>
       </c>
       <c r="F32">
-        <v>0.065</v>
+        <v>0.02666666666666667</v>
       </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33">
-        <v>2.505376344086022</v>
+        <v>1.862637362637363</v>
       </c>
       <c r="C33">
-        <v>0.07000000000000001</v>
+        <v>0.31</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33">
-        <v>0.865</v>
+        <v>0.58</v>
       </c>
       <c r="F33">
-        <v>0.065</v>
+        <v>0.02666666666666667</v>
       </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34">
-        <v>2.505376344086022</v>
+        <v>1.821989528795811</v>
       </c>
       <c r="C34">
-        <v>0.07000000000000001</v>
+        <v>0.2833333333333333</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>0.865</v>
+        <v>0.6066666666666667</v>
       </c>
       <c r="F34">
-        <v>0.065</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="35" spans="2:6">
       <c r="B35">
-        <v>2.505376344086022</v>
+        <v>1.84</v>
       </c>
       <c r="C35">
-        <v>0.07000000000000001</v>
+        <v>0.27</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>0.865</v>
+        <v>0.6333333333333333</v>
       </c>
       <c r="F35">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="36" spans="2:6">
       <c r="B36">
-        <v>2.505376344086022</v>
+        <v>1.831730769230769</v>
       </c>
       <c r="C36">
-        <v>0.07000000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36">
-        <v>0.865</v>
+        <v>0.66</v>
       </c>
       <c r="F36">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="37" spans="2:6">
       <c r="B37">
-        <v>2.492063492063492</v>
+        <v>1.81042654028436</v>
       </c>
       <c r="C37">
-        <v>0.055</v>
+        <v>0.2466666666666667</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37">
-        <v>0.88</v>
+        <v>0.67</v>
       </c>
       <c r="F37">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="38" spans="2:6">
       <c r="B38">
-        <v>2.492063492063492</v>
+        <v>1.784403669724771</v>
       </c>
       <c r="C38">
-        <v>0.055</v>
+        <v>0.2333333333333333</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38">
-        <v>0.88</v>
+        <v>0.6933333333333334</v>
       </c>
       <c r="F38">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="39" spans="2:6">
       <c r="B39">
-        <v>2.492063492063492</v>
+        <v>1.836283185840708</v>
       </c>
       <c r="C39">
-        <v>0.055</v>
+        <v>0.21</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39">
-        <v>0.88</v>
+        <v>0.72</v>
       </c>
       <c r="F39">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="40" spans="2:6">
       <c r="B40">
-        <v>2.489473684210526</v>
+        <v>1.807692307692308</v>
       </c>
       <c r="C40">
-        <v>0.05</v>
+        <v>0.1866666666666667</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40">
-        <v>0.885</v>
+        <v>0.7466666666666667</v>
       </c>
       <c r="F40">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="41" spans="2:6">
       <c r="B41">
-        <v>2.505208333333333</v>
+        <v>1.79253112033195</v>
       </c>
       <c r="C41">
-        <v>0.04</v>
+        <v>0.17</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41">
-        <v>0.895</v>
+        <v>0.77</v>
       </c>
       <c r="F41">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="42" spans="2:6">
       <c r="B42">
-        <v>2.556701030927835</v>
+        <v>1.766129032258065</v>
       </c>
       <c r="C42">
-        <v>0.03</v>
+        <v>0.1566666666666667</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42">
-        <v>0.905</v>
+        <v>0.7933333333333333</v>
       </c>
       <c r="F42">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="43" spans="2:6">
       <c r="B43">
-        <v>2.548717948717949</v>
+        <v>1.782608695652174</v>
       </c>
       <c r="C43">
-        <v>0.025</v>
+        <v>0.14</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43">
-        <v>0.91</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="F43">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="44" spans="2:6">
       <c r="B44">
-        <v>2.548717948717949</v>
+        <v>1.768339768339768</v>
       </c>
       <c r="C44">
-        <v>0.025</v>
+        <v>0.12</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>0.91</v>
+        <v>0.83</v>
       </c>
       <c r="F44">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="45" spans="2:6">
       <c r="B45">
-        <v>2.548717948717949</v>
+        <v>1.756653992395437</v>
       </c>
       <c r="C45">
-        <v>0.025</v>
+        <v>0.1066666666666667</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
       <c r="E45">
-        <v>0.91</v>
+        <v>0.8433333333333334</v>
       </c>
       <c r="F45">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="46" spans="2:6">
       <c r="B46">
-        <v>2.548717948717949</v>
+        <v>1.738805970149254</v>
       </c>
       <c r="C46">
-        <v>0.025</v>
+        <v>0.09</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46">
-        <v>0.91</v>
+        <v>0.86</v>
       </c>
       <c r="F46">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="47" spans="2:6">
       <c r="B47">
-        <v>2.535714285714286</v>
+        <v>1.730627306273063</v>
       </c>
       <c r="C47">
-        <v>0.02</v>
+        <v>0.08</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47">
-        <v>0.915</v>
+        <v>0.87</v>
       </c>
       <c r="F47">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="48" spans="2:6">
       <c r="B48">
-        <v>2.535714285714286</v>
+        <v>1.732600732600733</v>
       </c>
       <c r="C48">
-        <v>0.02</v>
+        <v>0.07333333333333333</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48">
-        <v>0.915</v>
+        <v>0.8766666666666667</v>
       </c>
       <c r="F48">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="49" spans="2:6">
       <c r="B49">
-        <v>2.535714285714286</v>
+        <v>1.723636363636364</v>
       </c>
       <c r="C49">
-        <v>0.02</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49">
-        <v>0.915</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="F49">
-        <v>0.065</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="50" spans="2:6">
       <c r="B50">
-        <v>2.515151515151515</v>
+        <v>1.714801444043321</v>
       </c>
       <c r="C50">
-        <v>0.01</v>
+        <v>0.06</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50">
-        <v>0.925</v>
+        <v>0.8866666666666667</v>
       </c>
       <c r="F50">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="51" spans="2:6">
       <c r="B51">
-        <v>2.515151515151515</v>
+        <v>1.707142857142857</v>
       </c>
       <c r="C51">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
       <c r="E51">
-        <v>0.925</v>
+        <v>0.8966666666666666</v>
       </c>
       <c r="F51">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="52" spans="2:6">
       <c r="B52">
-        <v>2.515151515151515</v>
+        <v>1.707142857142857</v>
       </c>
       <c r="C52">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52">
-        <v>0.925</v>
+        <v>0.8966666666666666</v>
       </c>
       <c r="F52">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="53" spans="2:6">
       <c r="B53">
-        <v>2.515151515151515</v>
+        <v>1.692579505300353</v>
       </c>
       <c r="C53">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53">
-        <v>0.925</v>
+        <v>0.9066666666666666</v>
       </c>
       <c r="F53">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="54" spans="2:6">
       <c r="B54">
-        <v>2.50251256281407</v>
+        <v>1.692579505300353</v>
       </c>
       <c r="C54">
-        <v>0.005</v>
+        <v>0.04</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54">
-        <v>0.93</v>
+        <v>0.9066666666666666</v>
       </c>
       <c r="F54">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="55" spans="2:6">
       <c r="B55">
-        <v>2.50251256281407</v>
+        <v>1.687719298245614</v>
       </c>
       <c r="C55">
-        <v>0.005</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55">
-        <v>0.93</v>
+        <v>0.9133333333333333</v>
       </c>
       <c r="F55">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="56" spans="2:6">
       <c r="B56">
-        <v>2.50251256281407</v>
+        <v>1.70383275261324</v>
       </c>
       <c r="C56">
-        <v>0.005</v>
+        <v>0.02666666666666667</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56">
-        <v>0.93</v>
+        <v>0.92</v>
       </c>
       <c r="F56">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="57" spans="2:6">
       <c r="B57">
-        <v>2.50251256281407</v>
+        <v>1.71875</v>
       </c>
       <c r="C57">
-        <v>0.005</v>
+        <v>0.02333333333333333</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57">
-        <v>0.93</v>
+        <v>0.9233333333333333</v>
       </c>
       <c r="F57">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="58" spans="2:6">
       <c r="B58">
-        <v>2.50251256281407</v>
+        <v>1.717241379310345</v>
       </c>
       <c r="C58">
-        <v>0.005</v>
+        <v>0.01666666666666667</v>
       </c>
       <c r="D58">
         <v>1</v>
@@ -1355,15 +1355,15 @@
         <v>0.93</v>
       </c>
       <c r="F58">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="59" spans="2:6">
       <c r="B59">
-        <v>2.50251256281407</v>
+        <v>1.717241379310345</v>
       </c>
       <c r="C59">
-        <v>0.005</v>
+        <v>0.01666666666666667</v>
       </c>
       <c r="D59">
         <v>1</v>
@@ -1372,15 +1372,15 @@
         <v>0.93</v>
       </c>
       <c r="F59">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="60" spans="2:6">
       <c r="B60">
-        <v>2.50251256281407</v>
+        <v>1.717241379310345</v>
       </c>
       <c r="C60">
-        <v>0.005</v>
+        <v>0.01666666666666667</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -1389,109 +1389,109 @@
         <v>0.93</v>
       </c>
       <c r="F60">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="61" spans="2:6">
       <c r="B61">
-        <v>2.50251256281407</v>
+        <v>1.711340206185567</v>
       </c>
       <c r="C61">
-        <v>0.005</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61">
-        <v>0.93</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="F61">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="62" spans="2:6">
       <c r="B62">
-        <v>2.50251256281407</v>
+        <v>1.711340206185567</v>
       </c>
       <c r="C62">
-        <v>0.005</v>
+        <v>0.01333333333333333</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62">
-        <v>0.93</v>
+        <v>0.9333333333333333</v>
       </c>
       <c r="F62">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="63" spans="2:6">
       <c r="B63">
-        <v>2.50251256281407</v>
+        <v>1.705479452054794</v>
       </c>
       <c r="C63">
-        <v>0.005</v>
+        <v>0.01</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63">
-        <v>0.93</v>
+        <v>0.9366666666666666</v>
       </c>
       <c r="F63">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="64" spans="2:6">
       <c r="B64">
-        <v>2.50251256281407</v>
+        <v>1.704081632653061</v>
       </c>
       <c r="C64">
-        <v>0.005</v>
+        <v>0.003333333333333334</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64">
-        <v>0.93</v>
+        <v>0.9433333333333334</v>
       </c>
       <c r="F64">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="65" spans="2:6">
       <c r="B65">
-        <v>2.50251256281407</v>
+        <v>1.704081632653061</v>
       </c>
       <c r="C65">
-        <v>0.005</v>
+        <v>0.003333333333333334</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65">
-        <v>0.93</v>
+        <v>0.9433333333333334</v>
       </c>
       <c r="F65">
-        <v>0.065</v>
+        <v>0.03666666666666667</v>
       </c>
     </row>
     <row r="66" spans="2:6">
       <c r="B66">
-        <v>2.50251256281407</v>
+        <v>0</v>
       </c>
       <c r="C66">
-        <v>0.005</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66">
-        <v>0.93</v>
+        <v>0</v>
       </c>
       <c r="F66">
-        <v>0.065</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="2:6">

</xml_diff>

<commit_message>
Kleinere Tests plus Neuintegration von r0
</commit_message>
<xml_diff>
--- a/Daten_Vergleich.xlsx
+++ b/Daten_Vergleich.xlsx
@@ -391,10 +391,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="B2">
-        <v>0</v>
+        <v>3.705882352941177</v>
       </c>
       <c r="C2">
-        <v>0.001538461538461538</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -408,13 +408,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="B3">
-        <v>0</v>
+        <v>3.705882352941177</v>
       </c>
       <c r="C3">
-        <v>0.002307692307692308</v>
+        <v>0.01</v>
       </c>
       <c r="D3">
-        <v>1.5</v>
+        <v>1.625</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -425,16 +425,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4">
-        <v>1</v>
+        <v>3.705882352941177</v>
       </c>
       <c r="C4">
-        <v>0.002307692307692308</v>
+        <v>0.01076923076923077</v>
       </c>
       <c r="D4">
-        <v>1.333333333333333</v>
+        <v>1.166666666666667</v>
       </c>
       <c r="E4">
-        <v>0.0007692307692307692</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -442,16 +442,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="B5">
-        <v>1</v>
+        <v>3.705882352941177</v>
       </c>
       <c r="C5">
-        <v>0.003076923076923077</v>
+        <v>0.01153846153846154</v>
       </c>
       <c r="D5">
-        <v>1.25</v>
+        <v>1.071428571428571</v>
       </c>
       <c r="E5">
-        <v>0.0007692307692307692</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -459,16 +459,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6">
-        <v>1</v>
+        <v>3.705882352941177</v>
       </c>
       <c r="C6">
-        <v>0.003846153846153846</v>
+        <v>0.01307692307692308</v>
       </c>
       <c r="D6">
-        <v>1.2</v>
+        <v>1.0625</v>
       </c>
       <c r="E6">
-        <v>0.0007692307692307692</v>
+        <v>0</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -476,13 +476,13 @@
     </row>
     <row r="7" spans="1:6">
       <c r="B7">
-        <v>1</v>
+        <v>3.705882352941177</v>
       </c>
       <c r="C7">
-        <v>0.007692307692307693</v>
+        <v>0.01307692307692308</v>
       </c>
       <c r="D7">
-        <v>1.1</v>
+        <v>1.058823529411765</v>
       </c>
       <c r="E7">
         <v>0.0007692307692307692</v>
@@ -493,16 +493,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="B8">
-        <v>1</v>
+        <v>2.193548387096774</v>
       </c>
       <c r="C8">
-        <v>0.01153846153846154</v>
+        <v>0.01461538461538462</v>
       </c>
       <c r="D8">
-        <v>1.066666666666667</v>
+        <v>1.05</v>
       </c>
       <c r="E8">
-        <v>0.0007692307692307692</v>
+        <v>0.001538461538461538</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -510,13 +510,13 @@
     </row>
     <row r="9" spans="1:6">
       <c r="B9">
-        <v>0.5</v>
+        <v>1.652173913043478</v>
       </c>
       <c r="C9">
-        <v>0.01307692307692308</v>
+        <v>0.01769230769230769</v>
       </c>
       <c r="D9">
-        <v>1.055555555555556</v>
+        <v>1.041666666666667</v>
       </c>
       <c r="E9">
         <v>0.001538461538461538</v>
@@ -527,16 +527,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="B10">
-        <v>0.6666666666666666</v>
+        <v>1.389830508474576</v>
       </c>
       <c r="C10">
-        <v>0.01384615384615385</v>
+        <v>0.01769230769230769</v>
       </c>
       <c r="D10">
-        <v>1.05</v>
+        <v>1.037037037037037</v>
       </c>
       <c r="E10">
-        <v>0.002307692307692308</v>
+        <v>0.003846153846153846</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -544,16 +544,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="B11">
-        <v>0.6666666666666666</v>
+        <v>1.412698412698413</v>
       </c>
       <c r="C11">
-        <v>0.01461538461538462</v>
+        <v>0.01846153846153846</v>
       </c>
       <c r="D11">
-        <v>1.047619047619048</v>
+        <v>1.033333333333333</v>
       </c>
       <c r="E11">
-        <v>0.002307692307692308</v>
+        <v>0.005384615384615384</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -561,2076 +561,2076 @@
     </row>
     <row r="12" spans="1:6">
       <c r="B12">
-        <v>1.4</v>
+        <v>1.411764705882353</v>
       </c>
       <c r="C12">
-        <v>0.01923076923076923</v>
+        <v>0.02</v>
       </c>
       <c r="D12">
-        <v>1.03448275862069</v>
+        <v>1.029411764705882</v>
       </c>
       <c r="E12">
-        <v>0.003846153846153846</v>
+        <v>0.006153846153846154</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>0.0007692307692307692</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13">
-        <v>1.166666666666667</v>
+        <v>1.381578947368421</v>
       </c>
       <c r="C13">
-        <v>0.02076923076923077</v>
+        <v>0.02461538461538462</v>
       </c>
       <c r="D13">
-        <v>1.03125</v>
+        <v>1.025</v>
       </c>
       <c r="E13">
-        <v>0.004615384615384616</v>
+        <v>0.006153846153846154</v>
       </c>
       <c r="F13">
-        <v>0</v>
+        <v>0.0007692307692307692</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14">
-        <v>1.444444444444444</v>
+        <v>1.365853658536585</v>
       </c>
       <c r="C14">
         <v>0.02307692307692308</v>
       </c>
       <c r="D14">
-        <v>1.026315789473684</v>
+        <v>1.024390243902439</v>
       </c>
       <c r="E14">
-        <v>0.006153846153846154</v>
+        <v>0.007692307692307693</v>
       </c>
       <c r="F14">
-        <v>0.0007692307692307692</v>
+        <v>0.001538461538461538</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15">
-        <v>1.272727272727273</v>
+        <v>1.314606741573034</v>
       </c>
       <c r="C15">
-        <v>0.02846153846153846</v>
+        <v>0.02230769230769231</v>
       </c>
       <c r="D15">
-        <v>1.021276595744681</v>
+        <v>1</v>
       </c>
       <c r="E15">
-        <v>0.007692307692307693</v>
+        <v>0.009230769230769232</v>
       </c>
       <c r="F15">
-        <v>0.0007692307692307692</v>
+        <v>0.001538461538461538</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16">
-        <v>1.272727272727273</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C16">
-        <v>0.02923076923076923</v>
+        <v>0.02846153846153846</v>
       </c>
       <c r="D16">
-        <v>1.020833333333333</v>
+        <v>1</v>
       </c>
       <c r="E16">
-        <v>0.007692307692307693</v>
+        <v>0.01076923076923077</v>
       </c>
       <c r="F16">
-        <v>0.0007692307692307692</v>
+        <v>0.001538461538461538</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17">
-        <v>1.533333333333333</v>
+        <v>1.333333333333333</v>
       </c>
       <c r="C17">
-        <v>0.03153846153846154</v>
+        <v>0.03384615384615385</v>
       </c>
       <c r="D17">
-        <v>1.018181818181818</v>
+        <v>1</v>
       </c>
       <c r="E17">
-        <v>0.01076923076923077</v>
+        <v>0.01153846153846154</v>
       </c>
       <c r="F17">
-        <v>0.0007692307692307692</v>
+        <v>0.001538461538461538</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18">
-        <v>1.533333333333333</v>
+        <v>1.419642857142857</v>
       </c>
       <c r="C18">
         <v>0.03769230769230769</v>
       </c>
       <c r="D18">
-        <v>1.015873015873016</v>
+        <v>1</v>
       </c>
       <c r="E18">
-        <v>0.01076923076923077</v>
+        <v>0.01384615384615385</v>
       </c>
       <c r="F18">
-        <v>0.0007692307692307692</v>
+        <v>0.002307692307692308</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19">
-        <v>1.5625</v>
+        <v>1.623931623931624</v>
       </c>
       <c r="C19">
-        <v>0.04307692307692308</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D19">
-        <v>1.014084507042254</v>
+        <v>1</v>
       </c>
       <c r="E19">
-        <v>0.01153846153846154</v>
+        <v>0.01769230769230769</v>
       </c>
       <c r="F19">
-        <v>0.0007692307692307692</v>
+        <v>0.002307692307692308</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20">
-        <v>1.25</v>
+        <v>1.7265625</v>
       </c>
       <c r="C20">
-        <v>0.04384615384615385</v>
+        <v>0.05230769230769231</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>0.01461538461538462</v>
+        <v>0.02</v>
       </c>
       <c r="F20">
-        <v>0.0007692307692307692</v>
+        <v>0.003076923076923077</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21">
-        <v>1.238095238095238</v>
+        <v>1.807142857142857</v>
       </c>
       <c r="C21">
-        <v>0.04769230769230769</v>
+        <v>0.05846153846153846</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>0.01538461538461539</v>
+        <v>0.02538461538461538</v>
       </c>
       <c r="F21">
-        <v>0.0007692307692307692</v>
+        <v>0.003846153846153846</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22">
-        <v>1.130434782608696</v>
+        <v>1.817610062893082</v>
       </c>
       <c r="C22">
-        <v>0.05538461538461539</v>
+        <v>0.06538461538461539</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>0.01692307692307692</v>
+        <v>0.02923076923076923</v>
       </c>
       <c r="F22">
-        <v>0.0007692307692307692</v>
+        <v>0.004615384615384616</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23">
-        <v>1.04</v>
+        <v>1.657894736842105</v>
       </c>
       <c r="C23">
-        <v>0.06538461538461539</v>
+        <v>0.06615384615384616</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>0.01846153846153846</v>
+        <v>0.03538461538461538</v>
       </c>
       <c r="F23">
-        <v>0.0007692307692307692</v>
+        <v>0.005384615384615384</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24">
-        <v>1</v>
+        <v>1.538461538461539</v>
       </c>
       <c r="C24">
-        <v>0.07307692307692308</v>
+        <v>0.07153846153846154</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>0.02076923076923077</v>
+        <v>0.04</v>
       </c>
       <c r="F24">
-        <v>0.0007692307692307692</v>
+        <v>0.006153846153846154</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25">
-        <v>1</v>
+        <v>1.462450592885375</v>
       </c>
       <c r="C25">
-        <v>0.07615384615384616</v>
+        <v>0.08153846153846153</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>0.02384615384615385</v>
+        <v>0.04230769230769231</v>
       </c>
       <c r="F25">
-        <v>0.001538461538461538</v>
+        <v>0.006153846153846154</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26">
-        <v>1.102564102564103</v>
+        <v>1.363321799307958</v>
       </c>
       <c r="C26">
-        <v>0.08076923076923077</v>
+        <v>0.08384615384615385</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>0.02769230769230769</v>
+        <v>0.04846153846153846</v>
       </c>
       <c r="F26">
-        <v>0.002307692307692308</v>
+        <v>0.006153846153846154</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27">
-        <v>1.2</v>
+        <v>1.393650793650794</v>
       </c>
       <c r="C27">
-        <v>0.08153846153846153</v>
+        <v>0.1007692307692308</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27">
-        <v>0.03615384615384615</v>
+        <v>0.05153846153846154</v>
       </c>
       <c r="F27">
-        <v>0.002307692307692308</v>
+        <v>0.006153846153846154</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28">
-        <v>1.333333333333333</v>
+        <v>1.423529411764706</v>
       </c>
       <c r="C28">
-        <v>0.08076923076923077</v>
+        <v>0.1061538461538462</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28">
-        <v>0.04153846153846154</v>
+        <v>0.0576923076923077</v>
       </c>
       <c r="F28">
-        <v>0.002307692307692308</v>
+        <v>0.006153846153846154</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29">
-        <v>1.265625</v>
+        <v>1.42972972972973</v>
       </c>
       <c r="C29">
-        <v>0.08307692307692308</v>
+        <v>0.1161538461538461</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29">
-        <v>0.04692307692307692</v>
+        <v>0.06230769230769231</v>
       </c>
       <c r="F29">
-        <v>0.002307692307692308</v>
+        <v>0.006923076923076923</v>
       </c>
     </row>
     <row r="30" spans="2:6">
       <c r="B30">
-        <v>1.1125</v>
+        <v>1.449238578680203</v>
       </c>
       <c r="C30">
-        <v>0.08</v>
+        <v>0.1161538461538461</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30">
-        <v>0.05846153846153846</v>
+        <v>0.06923076923076923</v>
       </c>
       <c r="F30">
-        <v>0.003076923076923077</v>
+        <v>0.006923076923076923</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31">
-        <v>1.111111111111111</v>
+        <v>1.369020501138952</v>
       </c>
       <c r="C31">
-        <v>0.07769230769230769</v>
+        <v>0.1238461538461538</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>0.06615384615384616</v>
+        <v>0.07153846153846154</v>
       </c>
       <c r="F31">
-        <v>0.003076923076923077</v>
+        <v>0.007692307692307693</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32">
-        <v>1.122448979591837</v>
+        <v>1.309917355371901</v>
       </c>
       <c r="C32">
-        <v>0.07538461538461538</v>
+        <v>0.1315384615384615</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>0.07230769230769231</v>
+        <v>0.07615384615384616</v>
       </c>
       <c r="F32">
-        <v>0.003076923076923077</v>
+        <v>0.007692307692307693</v>
       </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33">
-        <v>1.155339805825243</v>
+        <v>1.238185255198488</v>
       </c>
       <c r="C33">
-        <v>0.08384615384615385</v>
+        <v>0.1323076923076923</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33">
-        <v>0.07615384615384616</v>
+        <v>0.08461538461538462</v>
       </c>
       <c r="F33">
-        <v>0.003076923076923077</v>
+        <v>0.008461538461538461</v>
       </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34">
-        <v>1.089285714285714</v>
+        <v>1.192644483362522</v>
       </c>
       <c r="C34">
-        <v>0.08538461538461538</v>
+        <v>0.1361538461538462</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>0.08307692307692308</v>
+        <v>0.09538461538461539</v>
       </c>
       <c r="F34">
-        <v>0.003076923076923077</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="35" spans="2:6">
       <c r="B35">
-        <v>1.173553719008265</v>
+        <v>1.15973377703827</v>
       </c>
       <c r="C35">
-        <v>0.08538461538461538</v>
+        <v>0.1361538461538462</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>0.08923076923076922</v>
+        <v>0.1076923076923077</v>
       </c>
       <c r="F35">
-        <v>0.003846153846153846</v>
+        <v>0.01076923076923077</v>
       </c>
     </row>
     <row r="36" spans="2:6">
       <c r="B36">
-        <v>1.1640625</v>
+        <v>1.118296529968454</v>
       </c>
       <c r="C36">
-        <v>0.08384615384615385</v>
+        <v>0.1407692307692308</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36">
-        <v>0.09461538461538462</v>
+        <v>0.1207692307692308</v>
       </c>
       <c r="F36">
-        <v>0.003846153846153846</v>
+        <v>0.01153846153846154</v>
       </c>
     </row>
     <row r="37" spans="2:6">
       <c r="B37">
-        <v>1.140740740740741</v>
+        <v>1.105343511450382</v>
       </c>
       <c r="C37">
-        <v>0.08846153846153847</v>
+        <v>0.1438461538461538</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37">
-        <v>0.09846153846153846</v>
+        <v>0.13</v>
       </c>
       <c r="F37">
-        <v>0.005384615384615384</v>
+        <v>0.01153846153846154</v>
       </c>
     </row>
     <row r="38" spans="2:6">
       <c r="B38">
-        <v>1.142857142857143</v>
+        <v>1.095447870778267</v>
       </c>
       <c r="C38">
-        <v>0.08923076923076922</v>
+        <v>0.1530769230769231</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38">
-        <v>0.1061538461538462</v>
+        <v>0.1353846153846154</v>
       </c>
       <c r="F38">
-        <v>0.006923076923076923</v>
+        <v>0.01153846153846154</v>
       </c>
     </row>
     <row r="39" spans="2:6">
       <c r="B39">
-        <v>1.126666666666667</v>
+        <v>1.106169296987087</v>
       </c>
       <c r="C39">
-        <v>0.09461538461538462</v>
+        <v>0.1553846153846154</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39">
-        <v>0.1084615384615385</v>
+        <v>0.1484615384615385</v>
       </c>
       <c r="F39">
-        <v>0.006923076923076923</v>
+        <v>0.01230769230769231</v>
       </c>
     </row>
     <row r="40" spans="2:6">
       <c r="B40">
-        <v>1.103225806451613</v>
+        <v>1.124118476727785</v>
       </c>
       <c r="C40">
-        <v>0.1007692307692308</v>
+        <v>0.1607692307692308</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40">
-        <v>0.1115384615384615</v>
+        <v>0.1584615384615385</v>
       </c>
       <c r="F40">
-        <v>0.007692307692307693</v>
+        <v>0.01230769230769231</v>
       </c>
     </row>
     <row r="41" spans="2:6">
       <c r="B41">
-        <v>1.072289156626506</v>
+        <v>1.145027624309392</v>
       </c>
       <c r="C41">
-        <v>0.1046153846153846</v>
+        <v>0.1684615384615385</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41">
-        <v>0.1192307692307692</v>
+        <v>0.1669230769230769</v>
       </c>
       <c r="F41">
-        <v>0.008461538461538461</v>
+        <v>0.01307692307692308</v>
       </c>
     </row>
     <row r="42" spans="2:6">
       <c r="B42">
-        <v>1.063218390804598</v>
+        <v>1.140750670241287</v>
       </c>
       <c r="C42">
-        <v>0.1123076923076923</v>
+        <v>0.17</v>
       </c>
       <c r="D42">
         <v>1</v>
       </c>
       <c r="E42">
-        <v>0.1253846153846154</v>
+        <v>0.1807692307692308</v>
       </c>
       <c r="F42">
-        <v>0.008461538461538461</v>
+        <v>0.01384615384615385</v>
       </c>
     </row>
     <row r="43" spans="2:6">
       <c r="B43">
-        <v>1.088888888888889</v>
+        <v>1.138780804150454</v>
       </c>
       <c r="C43">
-        <v>0.1176923076923077</v>
+        <v>0.1761538461538462</v>
       </c>
       <c r="D43">
         <v>1</v>
       </c>
       <c r="E43">
-        <v>0.13</v>
+        <v>0.1938461538461538</v>
       </c>
       <c r="F43">
-        <v>0.008461538461538461</v>
+        <v>0.01461538461538462</v>
       </c>
     </row>
     <row r="44" spans="2:6">
       <c r="B44">
-        <v>1.105263157894737</v>
+        <v>1.130489335006273</v>
       </c>
       <c r="C44">
-        <v>0.12</v>
+        <v>0.1784615384615384</v>
       </c>
       <c r="D44">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>0.1369230769230769</v>
+        <v>0.2061538461538462</v>
       </c>
       <c r="F44">
-        <v>0.009230769230769232</v>
+        <v>0.01615384615384615</v>
       </c>
     </row>
     <row r="45" spans="2:6">
       <c r="B45">
-        <v>1.100502512562814</v>
+        <v>1.110977080820266</v>
       </c>
       <c r="C45">
-        <v>0.1230769230769231</v>
+        <v>0.1838461538461539</v>
       </c>
       <c r="D45">
         <v>1</v>
       </c>
       <c r="E45">
-        <v>0.1438461538461538</v>
+        <v>0.2138461538461539</v>
       </c>
       <c r="F45">
-        <v>0.009230769230769232</v>
+        <v>0.01692307692307692</v>
       </c>
     </row>
     <row r="46" spans="2:6">
       <c r="B46">
-        <v>1.086538461538461</v>
+        <v>1.09165687426557</v>
       </c>
       <c r="C46">
-        <v>0.1207692307692308</v>
+        <v>0.1761538461538462</v>
       </c>
       <c r="D46">
         <v>1</v>
       </c>
       <c r="E46">
-        <v>0.1484615384615385</v>
+        <v>0.2292307692307692</v>
       </c>
       <c r="F46">
-        <v>0.01153846153846154</v>
+        <v>0.02076923076923077</v>
       </c>
     </row>
     <row r="47" spans="2:6">
       <c r="B47">
-        <v>1.103139013452915</v>
+        <v>1.061503416856492</v>
       </c>
       <c r="C47">
-        <v>0.1246153846153846</v>
+        <v>0.1784615384615384</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47">
-        <v>0.16</v>
+        <v>0.2384615384615385</v>
       </c>
       <c r="F47">
-        <v>0.01153846153846154</v>
+        <v>0.02076923076923077</v>
       </c>
     </row>
     <row r="48" spans="2:6">
       <c r="B48">
-        <v>1.117647058823529</v>
+        <v>1.04661487236404</v>
       </c>
       <c r="C48">
-        <v>0.1253846153846154</v>
+        <v>0.1869230769230769</v>
       </c>
       <c r="D48">
         <v>1</v>
       </c>
       <c r="E48">
-        <v>0.1707692307692308</v>
+        <v>0.2453846153846154</v>
       </c>
       <c r="F48">
-        <v>0.01230769230769231</v>
+        <v>0.02076923076923077</v>
       </c>
     </row>
     <row r="49" spans="2:6">
       <c r="B49">
-        <v>1.088353413654618</v>
+        <v>1.036916395222584</v>
       </c>
       <c r="C49">
-        <v>0.1238461538461538</v>
+        <v>0.1930769230769231</v>
       </c>
       <c r="D49">
         <v>1</v>
       </c>
       <c r="E49">
-        <v>0.1784615384615384</v>
+        <v>0.2576923076923077</v>
       </c>
       <c r="F49">
-        <v>0.01307692307692308</v>
+        <v>0.02076923076923077</v>
       </c>
     </row>
     <row r="50" spans="2:6">
       <c r="B50">
-        <v>1.065384615384615</v>
+        <v>1.053821313240043</v>
       </c>
       <c r="C50">
-        <v>0.1215384615384615</v>
+        <v>0.1946153846153846</v>
       </c>
       <c r="D50">
         <v>1</v>
       </c>
       <c r="E50">
-        <v>0.1861538461538461</v>
+        <v>0.2669230769230769</v>
       </c>
       <c r="F50">
-        <v>0.01384615384615385</v>
+        <v>0.02384615384615385</v>
       </c>
     </row>
     <row r="51" spans="2:6">
       <c r="B51">
-        <v>1.070631970260223</v>
+        <v>1.063304721030043</v>
       </c>
       <c r="C51">
-        <v>0.1230769230769231</v>
+        <v>0.1876923076923077</v>
       </c>
       <c r="D51">
         <v>1</v>
       </c>
       <c r="E51">
-        <v>0.1930769230769231</v>
+        <v>0.2815384615384615</v>
       </c>
       <c r="F51">
-        <v>0.01384615384615385</v>
+        <v>0.02384615384615385</v>
       </c>
     </row>
     <row r="52" spans="2:6">
       <c r="B52">
-        <v>1.057142857142857</v>
+        <v>1.042417815482503</v>
       </c>
       <c r="C52">
-        <v>0.1223076923076923</v>
+        <v>0.1807692307692308</v>
       </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52">
-        <v>0.2015384615384615</v>
+        <v>0.2938461538461539</v>
       </c>
       <c r="F52">
-        <v>0.01384615384615385</v>
+        <v>0.02461538461538462</v>
       </c>
     </row>
     <row r="53" spans="2:6">
       <c r="B53">
-        <v>1.054794520547945</v>
+        <v>1.015706806282722</v>
       </c>
       <c r="C53">
-        <v>0.1192307692307692</v>
+        <v>0.1830769230769231</v>
       </c>
       <c r="D53">
         <v>1</v>
       </c>
       <c r="E53">
-        <v>0.2092307692307692</v>
+        <v>0.3007692307692308</v>
       </c>
       <c r="F53">
-        <v>0.01538461538461539</v>
+        <v>0.02538461538461538</v>
       </c>
     </row>
     <row r="54" spans="2:6">
       <c r="B54">
-        <v>1.067961165048544</v>
+        <v>0.9765066394279879</v>
       </c>
       <c r="C54">
-        <v>0.1184615384615385</v>
+        <v>0.1838461538461539</v>
       </c>
       <c r="D54">
         <v>1</v>
       </c>
       <c r="E54">
-        <v>0.2215384615384615</v>
+        <v>0.3115384615384615</v>
       </c>
       <c r="F54">
-        <v>0.01615384615384615</v>
+        <v>0.02538461538461538</v>
       </c>
     </row>
     <row r="55" spans="2:6">
       <c r="B55">
-        <v>1.063492063492063</v>
+        <v>0.9485368314833502</v>
       </c>
       <c r="C55">
-        <v>0.1284615384615385</v>
+        <v>0.1753846153846154</v>
       </c>
       <c r="D55">
         <v>1</v>
       </c>
       <c r="E55">
-        <v>0.2253846153846154</v>
+        <v>0.3238461538461538</v>
       </c>
       <c r="F55">
-        <v>0.01692307692307692</v>
+        <v>0.02615384615384615</v>
       </c>
     </row>
     <row r="56" spans="2:6">
       <c r="B56">
-        <v>1.069908814589666</v>
+        <v>0.9471007121057985</v>
       </c>
       <c r="C56">
-        <v>0.1230769230769231</v>
+        <v>0.1738461538461538</v>
       </c>
       <c r="D56">
         <v>1</v>
       </c>
       <c r="E56">
-        <v>0.2346153846153846</v>
+        <v>0.3330769230769231</v>
       </c>
       <c r="F56">
-        <v>0.01846153846153846</v>
+        <v>0.02615384615384615</v>
       </c>
     </row>
     <row r="57" spans="2:6">
       <c r="B57">
-        <v>1.061764705882353</v>
+        <v>0.9443298969072165</v>
       </c>
       <c r="C57">
-        <v>0.1284615384615385</v>
+        <v>0.1715384615384615</v>
       </c>
       <c r="D57">
         <v>1</v>
       </c>
       <c r="E57">
-        <v>0.2407692307692308</v>
+        <v>0.3415384615384615</v>
       </c>
       <c r="F57">
-        <v>0.02076923076923077</v>
+        <v>0.02615384615384615</v>
       </c>
     </row>
     <row r="58" spans="2:6">
       <c r="B58">
-        <v>1.048571428571428</v>
+        <v>0.9330543933054393</v>
       </c>
       <c r="C58">
-        <v>0.1269230769230769</v>
+        <v>0.1653846153846154</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58">
-        <v>0.2476923076923077</v>
+        <v>0.3546153846153846</v>
       </c>
       <c r="F58">
-        <v>0.02153846153846154</v>
+        <v>0.02692307692307692</v>
       </c>
     </row>
     <row r="59" spans="2:6">
       <c r="B59">
-        <v>1.036111111111111</v>
+        <v>0.9329787234042553</v>
       </c>
       <c r="C59">
-        <v>0.13</v>
+        <v>0.1638461538461538</v>
       </c>
       <c r="D59">
         <v>1</v>
       </c>
       <c r="E59">
-        <v>0.2553846153846154</v>
+        <v>0.3630769230769231</v>
       </c>
       <c r="F59">
-        <v>0.02153846153846154</v>
+        <v>0.02769230769230769</v>
       </c>
     </row>
     <row r="60" spans="2:6">
       <c r="B60">
-        <v>1.021390374331551</v>
+        <v>0.9226638023630505</v>
       </c>
       <c r="C60">
-        <v>0.1276923076923077</v>
+        <v>0.16</v>
       </c>
       <c r="D60">
         <v>1</v>
       </c>
       <c r="E60">
-        <v>0.2661538461538461</v>
+        <v>0.3715384615384615</v>
       </c>
       <c r="F60">
-        <v>0.02153846153846154</v>
+        <v>0.02846153846153846</v>
       </c>
     </row>
     <row r="61" spans="2:6">
       <c r="B61">
-        <v>1.02319587628866</v>
+        <v>0.9115720524017465</v>
       </c>
       <c r="C61">
-        <v>0.1238461538461538</v>
+        <v>0.1530769230769231</v>
       </c>
       <c r="D61">
         <v>1</v>
       </c>
       <c r="E61">
-        <v>0.2761538461538461</v>
+        <v>0.3830769230769231</v>
       </c>
       <c r="F61">
-        <v>0.02230769230769231</v>
+        <v>0.02923076923076923</v>
       </c>
     </row>
     <row r="62" spans="2:6">
       <c r="B62">
-        <v>1.014962593516209</v>
+        <v>0.9035874439461884</v>
       </c>
       <c r="C62">
-        <v>0.1207692307692308</v>
+        <v>0.1430769230769231</v>
       </c>
       <c r="D62">
         <v>1</v>
       </c>
       <c r="E62">
-        <v>0.2853846153846154</v>
+        <v>0.3976923076923077</v>
       </c>
       <c r="F62">
-        <v>0.02307692307692308</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="63" spans="2:6">
       <c r="B63">
-        <v>1.024271844660194</v>
+        <v>0.8711516533637401</v>
       </c>
       <c r="C63">
-        <v>0.1215384615384615</v>
+        <v>0.1315384615384615</v>
       </c>
       <c r="D63">
         <v>1</v>
       </c>
       <c r="E63">
-        <v>0.2938461538461539</v>
+        <v>0.4115384615384615</v>
       </c>
       <c r="F63">
-        <v>0.02307692307692308</v>
+        <v>0.03076923076923077</v>
       </c>
     </row>
     <row r="64" spans="2:6">
       <c r="B64">
-        <v>1.030805687203791</v>
+        <v>0.8428405122235157</v>
       </c>
       <c r="C64">
-        <v>0.1246153846153846</v>
+        <v>0.1292307692307692</v>
       </c>
       <c r="D64">
         <v>1</v>
       </c>
       <c r="E64">
-        <v>0.3007692307692308</v>
+        <v>0.4223076923076923</v>
       </c>
       <c r="F64">
-        <v>0.02384615384615385</v>
+        <v>0.03076923076923077</v>
       </c>
     </row>
     <row r="65" spans="2:6">
       <c r="B65">
-        <v>1.025287356321839</v>
+        <v>0.8203592814371259</v>
       </c>
       <c r="C65">
-        <v>0.1246153846153846</v>
+        <v>0.1230769230769231</v>
       </c>
       <c r="D65">
         <v>1</v>
       </c>
       <c r="E65">
-        <v>0.3107692307692307</v>
+        <v>0.43</v>
       </c>
       <c r="F65">
-        <v>0.02384615384615385</v>
+        <v>0.03153846153846154</v>
       </c>
     </row>
     <row r="66" spans="2:6">
       <c r="B66">
-        <v>0</v>
+        <v>0.8089330024813896</v>
       </c>
       <c r="C66">
-        <v>0</v>
+        <v>0.1176923076923077</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E66">
-        <v>0</v>
+        <v>0.4376923076923077</v>
       </c>
       <c r="F66">
-        <v>0</v>
+        <v>0.03307692307692308</v>
       </c>
     </row>
     <row r="67" spans="2:6">
       <c r="B67">
-        <v>0</v>
+        <v>0.8219895287958114</v>
       </c>
       <c r="C67">
-        <v>0</v>
+        <v>0.1130769230769231</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E67">
-        <v>0</v>
+        <v>0.4469230769230769</v>
       </c>
       <c r="F67">
-        <v>0</v>
+        <v>0.03307692307692308</v>
       </c>
     </row>
     <row r="68" spans="2:6">
       <c r="B68">
-        <v>0</v>
+        <v>0.8273480662983425</v>
       </c>
       <c r="C68">
-        <v>0</v>
+        <v>0.1069230769230769</v>
       </c>
       <c r="D68">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E68">
-        <v>0</v>
+        <v>0.4538461538461538</v>
       </c>
       <c r="F68">
-        <v>0</v>
+        <v>0.03384615384615385</v>
       </c>
     </row>
     <row r="69" spans="2:6">
       <c r="B69">
-        <v>0</v>
+        <v>0.8394160583941607</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>0.1046153846153846</v>
       </c>
       <c r="D69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E69">
-        <v>0</v>
+        <v>0.4607692307692308</v>
       </c>
       <c r="F69">
-        <v>0</v>
+        <v>0.03461538461538462</v>
       </c>
     </row>
     <row r="70" spans="2:6">
       <c r="B70">
-        <v>0</v>
+        <v>0.8374233128834357</v>
       </c>
       <c r="C70">
-        <v>0</v>
+        <v>0.09538461538461539</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E70">
-        <v>0</v>
+        <v>0.4723076923076923</v>
       </c>
       <c r="F70">
-        <v>0</v>
+        <v>0.03538461538461538</v>
       </c>
     </row>
     <row r="71" spans="2:6">
       <c r="B71">
-        <v>0</v>
+        <v>0.8343949044585988</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>0.09615384615384616</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E71">
-        <v>0</v>
+        <v>0.4769230769230769</v>
       </c>
       <c r="F71">
-        <v>0</v>
+        <v>0.03538461538461538</v>
       </c>
     </row>
     <row r="72" spans="2:6">
       <c r="B72">
-        <v>0</v>
+        <v>0.8414023372287146</v>
       </c>
       <c r="C72">
-        <v>0</v>
+        <v>0.09153846153846154</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E72">
-        <v>0</v>
+        <v>0.4846153846153846</v>
       </c>
       <c r="F72">
-        <v>0</v>
+        <v>0.03538461538461538</v>
       </c>
     </row>
     <row r="73" spans="2:6">
       <c r="B73">
-        <v>0</v>
+        <v>0.8347826086956521</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>0.08615384615384615</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E73">
-        <v>0</v>
+        <v>0.4907692307692308</v>
       </c>
       <c r="F73">
-        <v>0</v>
+        <v>0.03692307692307693</v>
       </c>
     </row>
     <row r="74" spans="2:6">
       <c r="B74">
-        <v>0</v>
+        <v>0.8479853479853479</v>
       </c>
       <c r="C74">
-        <v>0</v>
+        <v>0.0823076923076923</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E74">
-        <v>0</v>
+        <v>0.4946153846153846</v>
       </c>
       <c r="F74">
-        <v>0</v>
+        <v>0.03846153846153846</v>
       </c>
     </row>
     <row r="75" spans="2:6">
       <c r="B75">
-        <v>0</v>
+        <v>0.8396946564885496</v>
       </c>
       <c r="C75">
-        <v>0</v>
+        <v>0.07846153846153846</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E75">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F75">
-        <v>0</v>
+        <v>0.03923076923076923</v>
       </c>
     </row>
     <row r="76" spans="2:6">
       <c r="B76">
-        <v>0</v>
+        <v>0.8313492063492063</v>
       </c>
       <c r="C76">
-        <v>0</v>
+        <v>0.07538461538461538</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>0.5053846153846154</v>
       </c>
       <c r="F76">
-        <v>0</v>
+        <v>0.03923076923076923</v>
       </c>
     </row>
     <row r="77" spans="2:6">
       <c r="B77">
-        <v>0</v>
+        <v>0.8416666666666666</v>
       </c>
       <c r="C77">
-        <v>0</v>
+        <v>0.07461538461538461</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E77">
-        <v>0</v>
+        <v>0.5069230769230769</v>
       </c>
       <c r="F77">
-        <v>0</v>
+        <v>0.03923076923076923</v>
       </c>
     </row>
     <row r="78" spans="2:6">
       <c r="B78">
-        <v>0</v>
+        <v>0.8488120950323975</v>
       </c>
       <c r="C78">
-        <v>0</v>
+        <v>0.07384615384615385</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>0.5107692307692308</v>
       </c>
       <c r="F78">
-        <v>0</v>
+        <v>0.03923076923076923</v>
       </c>
     </row>
     <row r="79" spans="2:6">
       <c r="B79">
-        <v>0</v>
+        <v>0.8772727272727273</v>
       </c>
       <c r="C79">
-        <v>0</v>
+        <v>0.07307692307692308</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E79">
-        <v>0</v>
+        <v>0.5138461538461538</v>
       </c>
       <c r="F79">
-        <v>0</v>
+        <v>0.03923076923076923</v>
       </c>
     </row>
     <row r="80" spans="2:6">
       <c r="B80">
-        <v>0</v>
+        <v>0.9069212410501193</v>
       </c>
       <c r="C80">
-        <v>0</v>
+        <v>0.07076923076923076</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E80">
-        <v>0</v>
+        <v>0.5169230769230769</v>
       </c>
       <c r="F80">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="81" spans="2:6">
       <c r="B81">
-        <v>0</v>
+        <v>0.9158415841584159</v>
       </c>
       <c r="C81">
-        <v>0</v>
+        <v>0.06692307692307692</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E81">
-        <v>0</v>
+        <v>0.5215384615384615</v>
       </c>
       <c r="F81">
-        <v>0</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="82" spans="2:6">
       <c r="B82">
-        <v>0</v>
+        <v>0.9033078880407125</v>
       </c>
       <c r="C82">
-        <v>0</v>
+        <v>0.06230769230769231</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>0.5269230769230769</v>
       </c>
       <c r="F82">
-        <v>0</v>
+        <v>0.04153846153846154</v>
       </c>
     </row>
     <row r="83" spans="2:6">
       <c r="B83">
-        <v>0</v>
+        <v>0.8678756476683936</v>
       </c>
       <c r="C83">
-        <v>0</v>
+        <v>0.0576923076923077</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E83">
-        <v>0</v>
+        <v>0.5330769230769231</v>
       </c>
       <c r="F83">
-        <v>0</v>
+        <v>0.04153846153846154</v>
       </c>
     </row>
     <row r="84" spans="2:6">
       <c r="B84">
-        <v>0</v>
+        <v>0.8263157894736843</v>
       </c>
       <c r="C84">
-        <v>0</v>
+        <v>0.05461538461538461</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E84">
-        <v>0</v>
+        <v>0.5376923076923077</v>
       </c>
       <c r="F84">
-        <v>0</v>
+        <v>0.04230769230769231</v>
       </c>
     </row>
     <row r="85" spans="2:6">
       <c r="B85">
-        <v>0</v>
+        <v>0.7864864864864864</v>
       </c>
       <c r="C85">
-        <v>0</v>
+        <v>0.04923076923076923</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E85">
-        <v>0</v>
+        <v>0.5446153846153846</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>0.04230769230769231</v>
       </c>
     </row>
     <row r="86" spans="2:6">
       <c r="B86">
-        <v>0</v>
+        <v>0.76056338028169</v>
       </c>
       <c r="C86">
-        <v>0</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E86">
-        <v>0</v>
+        <v>0.5476923076923077</v>
       </c>
       <c r="F86">
-        <v>0</v>
+        <v>0.04307692307692308</v>
       </c>
     </row>
     <row r="87" spans="2:6">
       <c r="B87">
-        <v>0</v>
+        <v>0.7611940298507465</v>
       </c>
       <c r="C87">
-        <v>0</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E87">
-        <v>0</v>
+        <v>0.5507692307692308</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>0.04307692307692308</v>
       </c>
     </row>
     <row r="88" spans="2:6">
       <c r="B88">
-        <v>0</v>
+        <v>0.7770700636942676</v>
       </c>
       <c r="C88">
-        <v>0</v>
+        <v>0.04615384615384616</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E88">
-        <v>0</v>
+        <v>0.5523076923076923</v>
       </c>
       <c r="F88">
-        <v>0</v>
+        <v>0.04307692307692308</v>
       </c>
     </row>
     <row r="89" spans="2:6">
       <c r="B89">
-        <v>0</v>
+        <v>0.8316151202749142</v>
       </c>
       <c r="C89">
-        <v>0</v>
+        <v>0.04769230769230769</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E89">
-        <v>0</v>
+        <v>0.5523076923076923</v>
       </c>
       <c r="F89">
-        <v>0</v>
+        <v>0.04384615384615385</v>
       </c>
     </row>
     <row r="90" spans="2:6">
       <c r="B90">
-        <v>0</v>
+        <v>0.8851851851851853</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>0.04384615384615385</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E90">
-        <v>0</v>
+        <v>0.5576923076923077</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>0.04384615384615385</v>
       </c>
     </row>
     <row r="91" spans="2:6">
       <c r="B91">
-        <v>0</v>
+        <v>0.9137254901960784</v>
       </c>
       <c r="C91">
-        <v>0</v>
+        <v>0.04153846153846154</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E91">
-        <v>0</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>0.04384615384615385</v>
       </c>
     </row>
     <row r="92" spans="2:6">
       <c r="B92">
-        <v>0</v>
+        <v>0.9262295081967212</v>
       </c>
       <c r="C92">
-        <v>0</v>
+        <v>0.04076923076923077</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E92">
-        <v>0</v>
+        <v>0.5615384615384615</v>
       </c>
       <c r="F92">
-        <v>0</v>
+        <v>0.04384615384615385</v>
       </c>
     </row>
     <row r="93" spans="2:6">
       <c r="B93">
-        <v>0</v>
+        <v>0.871900826446281</v>
       </c>
       <c r="C93">
-        <v>0</v>
+        <v>0.03615384615384615</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E93">
-        <v>0</v>
+        <v>0.566923076923077</v>
       </c>
       <c r="F93">
-        <v>0</v>
+        <v>0.04461538461538461</v>
       </c>
     </row>
     <row r="94" spans="2:6">
       <c r="B94">
-        <v>0</v>
+        <v>0.8368200836820083</v>
       </c>
       <c r="C94">
-        <v>0</v>
+        <v>0.03538461538461538</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E94">
-        <v>0</v>
+        <v>0.5692307692307692</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>0.04461538461538461</v>
       </c>
     </row>
     <row r="95" spans="2:6">
       <c r="B95">
-        <v>0</v>
+        <v>0.8068669527896993</v>
       </c>
       <c r="C95">
-        <v>0</v>
+        <v>0.03230769230769231</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E95">
-        <v>0</v>
+        <v>0.5738461538461539</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>0.04461538461538461</v>
       </c>
     </row>
     <row r="96" spans="2:6">
       <c r="B96">
-        <v>0</v>
+        <v>0.7831858407079646</v>
       </c>
       <c r="C96">
-        <v>0</v>
+        <v>0.03230769230769231</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E96">
-        <v>0</v>
+        <v>0.5753846153846154</v>
       </c>
       <c r="F96">
-        <v>0</v>
+        <v>0.04461538461538461</v>
       </c>
     </row>
     <row r="97" spans="2:6">
       <c r="B97">
-        <v>0</v>
+        <v>0.8056872037914692</v>
       </c>
       <c r="C97">
-        <v>0</v>
+        <v>0.03076923076923077</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E97">
-        <v>0</v>
+        <v>0.5784615384615385</v>
       </c>
       <c r="F97">
-        <v>0</v>
+        <v>0.04461538461538461</v>
       </c>
     </row>
     <row r="98" spans="2:6">
       <c r="B98">
-        <v>0</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="C98">
-        <v>0</v>
+        <v>0.02923076923076923</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E98">
-        <v>0</v>
+        <v>0.5807692307692308</v>
       </c>
       <c r="F98">
-        <v>0</v>
+        <v>0.04461538461538461</v>
       </c>
     </row>
     <row r="99" spans="2:6">
       <c r="B99">
-        <v>0</v>
+        <v>0.8085106382978726</v>
       </c>
       <c r="C99">
-        <v>0</v>
+        <v>0.02461538461538462</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E99">
-        <v>0</v>
+        <v>0.5846153846153846</v>
       </c>
       <c r="F99">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="100" spans="2:6">
       <c r="B100">
-        <v>0</v>
+        <v>0.7740112994350282</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>0.02076923076923077</v>
       </c>
       <c r="D100">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E100">
-        <v>0</v>
+        <v>0.5884615384615385</v>
       </c>
       <c r="F100">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="101" spans="2:6">
       <c r="B101">
-        <v>0</v>
+        <v>0.7176470588235293</v>
       </c>
       <c r="C101">
-        <v>0</v>
+        <v>0.01923076923076923</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E101">
-        <v>0</v>
+        <v>0.59</v>
       </c>
       <c r="F101">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="102" spans="2:6">
       <c r="B102">
-        <v>0</v>
+        <v>0.6604938271604938</v>
       </c>
       <c r="C102">
-        <v>0</v>
+        <v>0.01769230769230769</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E102">
-        <v>0</v>
+        <v>0.5915384615384616</v>
       </c>
       <c r="F102">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="103" spans="2:6">
       <c r="B103">
-        <v>0</v>
+        <v>0.6184210526315789</v>
       </c>
       <c r="C103">
-        <v>0</v>
+        <v>0.01461538461538462</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E103">
-        <v>0</v>
+        <v>0.5946153846153847</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="104" spans="2:6">
       <c r="B104">
-        <v>0</v>
+        <v>0.6131386861313869</v>
       </c>
       <c r="C104">
-        <v>0</v>
+        <v>0.01307692307692308</v>
       </c>
       <c r="D104">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E104">
-        <v>0</v>
+        <v>0.5961538461538461</v>
       </c>
       <c r="F104">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="105" spans="2:6">
       <c r="B105">
-        <v>0</v>
+        <v>0.6229508196721311</v>
       </c>
       <c r="C105">
-        <v>0</v>
+        <v>0.01307692307692308</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E105">
-        <v>0</v>
+        <v>0.5961538461538461</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="106" spans="2:6">
       <c r="B106">
-        <v>0</v>
+        <v>0.6355140186915887</v>
       </c>
       <c r="C106">
-        <v>0</v>
+        <v>0.01153846153846154</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E106">
-        <v>0</v>
+        <v>0.5976923076923077</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="107" spans="2:6">
       <c r="B107">
-        <v>0</v>
+        <v>0.6382978723404255</v>
       </c>
       <c r="C107">
-        <v>0</v>
+        <v>0.008461538461538461</v>
       </c>
       <c r="D107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E107">
-        <v>0</v>
+        <v>0.6007692307692307</v>
       </c>
       <c r="F107">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="108" spans="2:6">
       <c r="B108">
-        <v>0</v>
+        <v>0.6190476190476191</v>
       </c>
       <c r="C108">
-        <v>0</v>
+        <v>0.006923076923076923</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E108">
-        <v>0</v>
+        <v>0.6023076923076923</v>
       </c>
       <c r="F108">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="109" spans="2:6">
       <c r="B109">
-        <v>0</v>
+        <v>0.5526315789473685</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>0.005384615384615384</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109">
-        <v>0</v>
+        <v>0.6038461538461538</v>
       </c>
       <c r="F109">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="110" spans="2:6">
       <c r="B110">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="C110">
-        <v>0</v>
+        <v>0.005384615384615384</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E110">
-        <v>0</v>
+        <v>0.6038461538461538</v>
       </c>
       <c r="F110">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="111" spans="2:6">
       <c r="B111">
-        <v>0</v>
+        <v>0.4833333333333334</v>
       </c>
       <c r="C111">
-        <v>0</v>
+        <v>0.004615384615384616</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111">
-        <v>0</v>
+        <v>0.6046153846153847</v>
       </c>
       <c r="F111">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="112" spans="2:6">
       <c r="B112">
-        <v>0</v>
+        <v>0.4807692307692307</v>
       </c>
       <c r="C112">
-        <v>0</v>
+        <v>0.003846153846153846</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112">
-        <v>0</v>
+        <v>0.6053846153846154</v>
       </c>
       <c r="F112">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="113" spans="2:6">
       <c r="B113">
-        <v>0</v>
+        <v>0.5476190476190476</v>
       </c>
       <c r="C113">
-        <v>0</v>
+        <v>0.003846153846153846</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113">
-        <v>0</v>
+        <v>0.6053846153846154</v>
       </c>
       <c r="F113">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="114" spans="2:6">
       <c r="B114">
-        <v>0</v>
+        <v>0.6176470588235294</v>
       </c>
       <c r="C114">
-        <v>0</v>
+        <v>0.003846153846153846</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E114">
-        <v>0</v>
+        <v>0.6053846153846154</v>
       </c>
       <c r="F114">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="115" spans="2:6">
       <c r="B115">
-        <v>0</v>
+        <v>0.689655172413793</v>
       </c>
       <c r="C115">
-        <v>0</v>
+        <v>0.003846153846153846</v>
       </c>
       <c r="D115">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E115">
-        <v>0</v>
+        <v>0.6053846153846154</v>
       </c>
       <c r="F115">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="116" spans="2:6">
       <c r="B116">
-        <v>0</v>
+        <v>0.7600000000000001</v>
       </c>
       <c r="C116">
-        <v>0</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="D116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E116">
-        <v>0</v>
+        <v>0.6061538461538462</v>
       </c>
       <c r="F116">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="117" spans="2:6">
       <c r="B117">
-        <v>0</v>
+        <v>0.7826086956521739</v>
       </c>
       <c r="C117">
-        <v>0</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="D117">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E117">
-        <v>0</v>
+        <v>0.6061538461538462</v>
       </c>
       <c r="F117">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="118" spans="2:6">
       <c r="B118">
-        <v>0</v>
+        <v>0.8095238095238094</v>
       </c>
       <c r="C118">
-        <v>0</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E118">
-        <v>0</v>
+        <v>0.6061538461538462</v>
       </c>
       <c r="F118">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="119" spans="2:6">
       <c r="B119">
-        <v>0</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="C119">
-        <v>0</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="D119">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>0.6061538461538462</v>
       </c>
       <c r="F119">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="120" spans="2:6">
       <c r="B120">
-        <v>0</v>
+        <v>0.8421052631578947</v>
       </c>
       <c r="C120">
-        <v>0</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E120">
-        <v>0</v>
+        <v>0.6061538461538462</v>
       </c>
       <c r="F120">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="121" spans="2:6">
       <c r="B121">
-        <v>0</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="C121">
-        <v>0</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="D121">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E121">
-        <v>0</v>
+        <v>0.6061538461538462</v>
       </c>
       <c r="F121">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="122" spans="2:6">
       <c r="B122">
-        <v>0</v>
+        <v>0.8823529411764707</v>
       </c>
       <c r="C122">
-        <v>0</v>
+        <v>0.002307692307692308</v>
       </c>
       <c r="D122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E122">
-        <v>0</v>
+        <v>0.6069230769230769</v>
       </c>
       <c r="F122">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="123" spans="2:6">
       <c r="B123">
-        <v>0</v>
+        <v>0.8750000000000001</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>0.002307692307692308</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E123">
-        <v>0</v>
+        <v>0.6069230769230769</v>
       </c>
       <c r="F123">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="124" spans="2:6">
       <c r="B124">
-        <v>0</v>
+        <v>0.8125000000000001</v>
       </c>
       <c r="C124">
-        <v>0</v>
+        <v>0.002307692307692308</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E124">
-        <v>0</v>
+        <v>0.6069230769230769</v>
       </c>
       <c r="F124">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="125" spans="2:6">
       <c r="B125">
-        <v>0</v>
+        <v>0.7500000000000001</v>
       </c>
       <c r="C125">
-        <v>0</v>
+        <v>0.002307692307692308</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E125">
-        <v>0</v>
+        <v>0.6069230769230769</v>
       </c>
       <c r="F125">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="126" spans="2:6">
       <c r="B126">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="C126">
-        <v>0</v>
+        <v>0.002307692307692308</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E126">
-        <v>0</v>
+        <v>0.6069230769230769</v>
       </c>
       <c r="F126">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="127" spans="2:6">
       <c r="B127">
-        <v>0</v>
+        <v>0.8571428571428571</v>
       </c>
       <c r="C127">
-        <v>0</v>
+        <v>0.002307692307692308</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E127">
-        <v>0</v>
+        <v>0.6069230769230769</v>
       </c>
       <c r="F127">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="128" spans="2:6">
       <c r="B128">
-        <v>0</v>
+        <v>0.8461538461538459</v>
       </c>
       <c r="C128">
-        <v>0</v>
+        <v>0.001538461538461538</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E128">
-        <v>0</v>
+        <v>0.6076923076923076</v>
       </c>
       <c r="F128">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="129" spans="2:6">
       <c r="B129">
-        <v>0</v>
+        <v>0.8333333333333333</v>
       </c>
       <c r="C129">
-        <v>0</v>
+        <v>0.001538461538461538</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E129">
-        <v>0</v>
+        <v>0.6076923076923076</v>
       </c>
       <c r="F129">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="130" spans="2:6">
       <c r="B130">
-        <v>0</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>0.0007692307692307692</v>
       </c>
       <c r="D130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E130">
-        <v>0</v>
+        <v>0.6084615384615385</v>
       </c>
       <c r="F130">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="131" spans="2:6">
       <c r="B131">
-        <v>0</v>
+        <v>0.4999999999999999</v>
       </c>
       <c r="C131">
-        <v>0</v>
+        <v>0.0007692307692307692</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E131">
-        <v>0</v>
+        <v>0.6084615384615385</v>
       </c>
       <c r="F131">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="132" spans="2:6">
       <c r="B132">
-        <v>0</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="C132">
-        <v>0</v>
+        <v>0.0007692307692307692</v>
       </c>
       <c r="D132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E132">
-        <v>0</v>
+        <v>0.6084615384615385</v>
       </c>
       <c r="F132">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="133" spans="2:6">
       <c r="B133">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="C133">
-        <v>0</v>
+        <v>0.0007692307692307692</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E133">
-        <v>0</v>
+        <v>0.6084615384615385</v>
       </c>
       <c r="F133">
-        <v>0</v>
+        <v>0.04538461538461538</v>
       </c>
     </row>
     <row r="134" spans="2:6">

</xml_diff>

<commit_message>
Auslagern GUI als Funktion
</commit_message>
<xml_diff>
--- a/Daten_Vergleich.xlsx
+++ b/Daten_Vergleich.xlsx
@@ -391,7 +391,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="B2">
-        <v>3.705882352941177</v>
+        <v>4.500000000000001</v>
       </c>
       <c r="C2">
         <v>0.003076923076923077</v>
@@ -408,13 +408,13 @@
     </row>
     <row r="3" spans="1:6">
       <c r="B3">
-        <v>3.705882352941177</v>
+        <v>4.500000000000001</v>
       </c>
       <c r="C3">
-        <v>0.01</v>
+        <v>0.01076923076923077</v>
       </c>
       <c r="D3">
-        <v>1.625</v>
+        <v>1.555555555555556</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -425,13 +425,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="B4">
-        <v>3.705882352941177</v>
+        <v>4.500000000000001</v>
       </c>
       <c r="C4">
-        <v>0.01076923076923077</v>
+        <v>0.01153846153846154</v>
       </c>
       <c r="D4">
-        <v>1.166666666666667</v>
+        <v>1.25</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -442,16 +442,16 @@
     </row>
     <row r="5" spans="1:6">
       <c r="B5">
-        <v>3.705882352941177</v>
+        <v>4.500000000000001</v>
       </c>
       <c r="C5">
-        <v>0.01153846153846154</v>
+        <v>0.01615384615384615</v>
       </c>
       <c r="D5">
-        <v>1.071428571428571</v>
+        <v>1.157894736842105</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.0007692307692307692</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -459,16 +459,16 @@
     </row>
     <row r="6" spans="1:6">
       <c r="B6">
-        <v>3.705882352941177</v>
+        <v>4.500000000000001</v>
       </c>
       <c r="C6">
-        <v>0.01307692307692308</v>
+        <v>0.01538461538461539</v>
       </c>
       <c r="D6">
-        <v>1.0625</v>
+        <v>1.1</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>0.001538461538461538</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -476,16 +476,16 @@
     </row>
     <row r="7" spans="1:6">
       <c r="B7">
-        <v>3.705882352941177</v>
+        <v>4.500000000000001</v>
       </c>
       <c r="C7">
-        <v>0.01307692307692308</v>
+        <v>0.01923076923076923</v>
       </c>
       <c r="D7">
-        <v>1.058823529411765</v>
+        <v>1.08</v>
       </c>
       <c r="E7">
-        <v>0.0007692307692307692</v>
+        <v>0.001538461538461538</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -493,16 +493,16 @@
     </row>
     <row r="8" spans="1:6">
       <c r="B8">
-        <v>2.193548387096774</v>
+        <v>2.90909090909091</v>
       </c>
       <c r="C8">
-        <v>0.01461538461538462</v>
+        <v>0.02307692307692308</v>
       </c>
       <c r="D8">
-        <v>1.05</v>
+        <v>1.03030303030303</v>
       </c>
       <c r="E8">
-        <v>0.001538461538461538</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -510,16 +510,16 @@
     </row>
     <row r="9" spans="1:6">
       <c r="B9">
-        <v>1.652173913043478</v>
+        <v>2.111111111111111</v>
       </c>
       <c r="C9">
-        <v>0.01769230769230769</v>
+        <v>0.03</v>
       </c>
       <c r="D9">
-        <v>1.041666666666667</v>
+        <v>1.023809523809524</v>
       </c>
       <c r="E9">
-        <v>0.001538461538461538</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -527,16 +527,16 @@
     </row>
     <row r="10" spans="1:6">
       <c r="B10">
-        <v>1.389830508474576</v>
+        <v>2.085714285714286</v>
       </c>
       <c r="C10">
-        <v>0.01769230769230769</v>
+        <v>0.04</v>
       </c>
       <c r="D10">
-        <v>1.037037037037037</v>
+        <v>1.018181818181818</v>
       </c>
       <c r="E10">
-        <v>0.003846153846153846</v>
+        <v>0.003076923076923077</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -544,16 +544,16 @@
     </row>
     <row r="11" spans="1:6">
       <c r="B11">
-        <v>1.412698412698413</v>
+        <v>2.259259259259259</v>
       </c>
       <c r="C11">
-        <v>0.01846153846153846</v>
+        <v>0.04769230769230769</v>
       </c>
       <c r="D11">
-        <v>1.033333333333333</v>
+        <v>1.014925373134328</v>
       </c>
       <c r="E11">
-        <v>0.005384615384615384</v>
+        <v>0.004615384615384616</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -561,16 +561,16 @@
     </row>
     <row r="12" spans="1:6">
       <c r="B12">
-        <v>1.411764705882353</v>
+        <v>2.354166666666667</v>
       </c>
       <c r="C12">
-        <v>0.02</v>
+        <v>0.05615384615384615</v>
       </c>
       <c r="D12">
-        <v>1.029411764705882</v>
+        <v>1.01219512195122</v>
       </c>
       <c r="E12">
-        <v>0.006153846153846154</v>
+        <v>0.006923076923076923</v>
       </c>
       <c r="F12">
         <v>0.0007692307692307692</v>
@@ -578,288 +578,288 @@
     </row>
     <row r="13" spans="1:6">
       <c r="B13">
-        <v>1.381578947368421</v>
+        <v>2.37719298245614</v>
       </c>
       <c r="C13">
-        <v>0.02461538461538462</v>
+        <v>0.06461538461538462</v>
       </c>
       <c r="D13">
-        <v>1.025</v>
+        <v>1.010526315789474</v>
       </c>
       <c r="E13">
-        <v>0.006153846153846154</v>
+        <v>0.007692307692307693</v>
       </c>
       <c r="F13">
-        <v>0.0007692307692307692</v>
+        <v>0.001538461538461538</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14">
-        <v>1.365853658536585</v>
+        <v>2.178082191780822</v>
       </c>
       <c r="C14">
-        <v>0.02307692307692308</v>
+        <v>0.07615384615384616</v>
       </c>
       <c r="D14">
-        <v>1.024390243902439</v>
+        <v>1.008620689655172</v>
       </c>
       <c r="E14">
-        <v>0.007692307692307693</v>
+        <v>0.2038461538461538</v>
       </c>
       <c r="F14">
-        <v>0.001538461538461538</v>
+        <v>0.002307692307692308</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15">
-        <v>1.314606741573034</v>
+        <v>1.989071038251367</v>
       </c>
       <c r="C15">
-        <v>0.02230769230769231</v>
+        <v>0.08307692307692308</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>1.007692307692308</v>
       </c>
       <c r="E15">
-        <v>0.009230769230769232</v>
+        <v>0.2069230769230769</v>
       </c>
       <c r="F15">
-        <v>0.001538461538461538</v>
+        <v>0.003076923076923077</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16">
-        <v>1.333333333333333</v>
+        <v>1.792035398230089</v>
       </c>
       <c r="C16">
-        <v>0.02846153846153846</v>
+        <v>0.08769230769230769</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>1.007142857142857</v>
       </c>
       <c r="E16">
-        <v>0.01076923076923077</v>
+        <v>0.2092307692307692</v>
       </c>
       <c r="F16">
-        <v>0.001538461538461538</v>
+        <v>0.003846153846153846</v>
       </c>
     </row>
     <row r="17" spans="2:6">
       <c r="B17">
-        <v>1.333333333333333</v>
+        <v>1.608856088560886</v>
       </c>
       <c r="C17">
-        <v>0.03384615384615385</v>
+        <v>0.08846153846153847</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>1.006622516556291</v>
       </c>
       <c r="E17">
-        <v>0.01153846153846154</v>
+        <v>0.2169230769230769</v>
       </c>
       <c r="F17">
-        <v>0.001538461538461538</v>
+        <v>0.003846153846153846</v>
       </c>
     </row>
     <row r="18" spans="2:6">
       <c r="B18">
-        <v>1.419642857142857</v>
+        <v>1.437106918238994</v>
       </c>
       <c r="C18">
-        <v>0.03769230769230769</v>
+        <v>0.09230769230769231</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>1.006134969325153</v>
       </c>
       <c r="E18">
-        <v>0.01384615384615385</v>
+        <v>0.2223076923076923</v>
       </c>
       <c r="F18">
-        <v>0.002307692307692308</v>
+        <v>0.003846153846153846</v>
       </c>
     </row>
     <row r="19" spans="2:6">
       <c r="B19">
-        <v>1.623931623931624</v>
+        <v>1.263736263736264</v>
       </c>
       <c r="C19">
-        <v>0.04615384615384616</v>
+        <v>0.08538461538461538</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>1.005917159763314</v>
       </c>
       <c r="E19">
-        <v>0.01769230769230769</v>
+        <v>0.2323076923076923</v>
       </c>
       <c r="F19">
-        <v>0.002307692307692308</v>
+        <v>0.005384615384615384</v>
       </c>
     </row>
     <row r="20" spans="2:6">
       <c r="B20">
-        <v>1.7265625</v>
+        <v>1.135802469135803</v>
       </c>
       <c r="C20">
-        <v>0.05230769230769231</v>
+        <v>0.08769230769230769</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
-        <v>0.02</v>
+        <v>0.2384615384615385</v>
       </c>
       <c r="F20">
-        <v>0.003076923076923077</v>
+        <v>0.005384615384615384</v>
       </c>
     </row>
     <row r="21" spans="2:6">
       <c r="B21">
-        <v>1.807142857142857</v>
+        <v>1.059633027522936</v>
       </c>
       <c r="C21">
-        <v>0.05846153846153846</v>
+        <v>0.09</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21">
-        <v>0.02538461538461538</v>
+        <v>0.2430769230769231</v>
       </c>
       <c r="F21">
-        <v>0.003846153846153846</v>
+        <v>0.006153846153846154</v>
       </c>
     </row>
     <row r="22" spans="2:6">
       <c r="B22">
-        <v>1.817610062893082</v>
+        <v>1.006564551422319</v>
       </c>
       <c r="C22">
-        <v>0.06538461538461539</v>
+        <v>0.09076923076923077</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22">
-        <v>0.02923076923076923</v>
+        <v>0.2492307692307692</v>
       </c>
       <c r="F22">
-        <v>0.004615384615384616</v>
+        <v>0.006923076923076923</v>
       </c>
     </row>
     <row r="23" spans="2:6">
       <c r="B23">
-        <v>1.657894736842105</v>
+        <v>1.013043478260869</v>
       </c>
       <c r="C23">
-        <v>0.06615384615384616</v>
+        <v>0.09</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23">
-        <v>0.03538461538461538</v>
+        <v>0.2553846153846154</v>
       </c>
       <c r="F23">
-        <v>0.005384615384615384</v>
+        <v>0.006923076923076923</v>
       </c>
     </row>
     <row r="24" spans="2:6">
       <c r="B24">
-        <v>1.538461538461539</v>
+        <v>0.8826086956521738</v>
       </c>
       <c r="C24">
-        <v>0.07153846153846154</v>
+        <v>0.04153846153846154</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24">
-        <v>0.04</v>
+        <v>0.3092307692307693</v>
       </c>
       <c r="F24">
-        <v>0.006153846153846154</v>
+        <v>0.006923076923076923</v>
       </c>
     </row>
     <row r="25" spans="2:6">
       <c r="B25">
-        <v>1.462450592885375</v>
+        <v>0.738095238095238</v>
       </c>
       <c r="C25">
-        <v>0.08153846153846153</v>
+        <v>0.04</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
-        <v>0.04230769230769231</v>
+        <v>0.3138461538461538</v>
       </c>
       <c r="F25">
-        <v>0.006153846153846154</v>
+        <v>0.006923076923076923</v>
       </c>
     </row>
     <row r="26" spans="2:6">
       <c r="B26">
-        <v>1.363321799307958</v>
+        <v>0.6173913043478261</v>
       </c>
       <c r="C26">
-        <v>0.08384615384615385</v>
+        <v>0.04692307692307692</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
-        <v>0.04846153846153846</v>
+        <v>0.3146153846153846</v>
       </c>
       <c r="F26">
-        <v>0.006153846153846154</v>
+        <v>0.006923076923076923</v>
       </c>
     </row>
     <row r="27" spans="2:6">
       <c r="B27">
-        <v>1.393650793650794</v>
+        <v>0.4914163090128756</v>
       </c>
       <c r="C27">
-        <v>0.1007692307692308</v>
+        <v>0.04769230769230769</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27">
-        <v>0.05153846153846154</v>
+        <v>0.3161538461538462</v>
       </c>
       <c r="F27">
-        <v>0.006153846153846154</v>
+        <v>0.006923076923076923</v>
       </c>
     </row>
     <row r="28" spans="2:6">
       <c r="B28">
-        <v>1.423529411764706</v>
+        <v>0.5886699507389164</v>
       </c>
       <c r="C28">
-        <v>0.1061538461538462</v>
+        <v>0.04923076923076923</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28">
-        <v>0.0576923076923077</v>
+        <v>0.3192307692307692</v>
       </c>
       <c r="F28">
-        <v>0.006153846153846154</v>
+        <v>0.006923076923076923</v>
       </c>
     </row>
     <row r="29" spans="2:6">
       <c r="B29">
-        <v>1.42972972972973</v>
+        <v>0.7331378299120235</v>
       </c>
       <c r="C29">
-        <v>0.1161538461538461</v>
+        <v>0.04846153846153846</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29">
-        <v>0.06230769230769231</v>
+        <v>0.3230769230769231</v>
       </c>
       <c r="F29">
         <v>0.006923076923076923</v>
@@ -867,1770 +867,1770 @@
     </row>
     <row r="30" spans="2:6">
       <c r="B30">
-        <v>1.449238578680203</v>
+        <v>0.8732394366197184</v>
       </c>
       <c r="C30">
-        <v>0.1161538461538461</v>
+        <v>0.04538461538461538</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30">
-        <v>0.06923076923076923</v>
+        <v>0.3276923076923077</v>
       </c>
       <c r="F30">
-        <v>0.006923076923076923</v>
+        <v>0.008461538461538461</v>
       </c>
     </row>
     <row r="31" spans="2:6">
       <c r="B31">
-        <v>1.369020501138952</v>
+        <v>1.061135371179039</v>
       </c>
       <c r="C31">
-        <v>0.1238461538461538</v>
+        <v>0.04384615384615385</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31">
-        <v>0.07153846153846154</v>
+        <v>0.33</v>
       </c>
       <c r="F31">
-        <v>0.007692307692307693</v>
+        <v>0.008461538461538461</v>
       </c>
     </row>
     <row r="32" spans="2:6">
       <c r="B32">
-        <v>1.309917355371901</v>
+        <v>0.9581589958158996</v>
       </c>
       <c r="C32">
-        <v>0.1315384615384615</v>
+        <v>0.03846153846153846</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>0.07615384615384616</v>
+        <v>0.3361538461538461</v>
       </c>
       <c r="F32">
-        <v>0.007692307692307693</v>
+        <v>0.008461538461538461</v>
       </c>
     </row>
     <row r="33" spans="2:6">
       <c r="B33">
-        <v>1.238185255198488</v>
+        <v>0.868</v>
       </c>
       <c r="C33">
-        <v>0.1323076923076923</v>
+        <v>0.03923076923076923</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33">
-        <v>0.08461538461538462</v>
+        <v>0.3376923076923077</v>
       </c>
       <c r="F33">
-        <v>0.008461538461538461</v>
+        <v>0.009230769230769232</v>
       </c>
     </row>
     <row r="34" spans="2:6">
       <c r="B34">
-        <v>1.192644483362522</v>
+        <v>0.8346774193548387</v>
       </c>
       <c r="C34">
-        <v>0.1361538461538462</v>
+        <v>0.03769230769230769</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>0.09538461538461539</v>
+        <v>0.4607692307692308</v>
       </c>
       <c r="F34">
-        <v>0.01</v>
+        <v>0.009230769230769232</v>
       </c>
     </row>
     <row r="35" spans="2:6">
       <c r="B35">
-        <v>1.15973377703827</v>
+        <v>0.8230452674897121</v>
       </c>
       <c r="C35">
-        <v>0.1361538461538462</v>
+        <v>0.03846153846153846</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>0.1076923076923077</v>
+        <v>0.6453846153846153</v>
       </c>
       <c r="F35">
-        <v>0.01076923076923077</v>
+        <v>0.009230769230769232</v>
       </c>
     </row>
     <row r="36" spans="2:6">
       <c r="B36">
-        <v>1.118296529968454</v>
+        <v>0.8602620087336245</v>
       </c>
       <c r="C36">
-        <v>0.1407692307692308</v>
+        <v>0.03615384615384615</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36">
-        <v>0.1207692307692308</v>
+        <v>0.6476923076923077</v>
       </c>
       <c r="F36">
-        <v>0.01153846153846154</v>
+        <v>0.009230769230769232</v>
       </c>
     </row>
     <row r="37" spans="2:6">
       <c r="B37">
-        <v>1.105343511450382</v>
+        <v>0.8294930875576038</v>
       </c>
       <c r="C37">
-        <v>0.1438461538461538</v>
+        <v>0.02615384615384615</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="E37">
-        <v>0.13</v>
+        <v>0.6584615384615384</v>
       </c>
       <c r="F37">
-        <v>0.01153846153846154</v>
+        <v>0.009230769230769232</v>
       </c>
     </row>
     <row r="38" spans="2:6">
       <c r="B38">
-        <v>1.095447870778267</v>
+        <v>0.6908212560386473</v>
       </c>
       <c r="C38">
-        <v>0.1530769230769231</v>
+        <v>0.009230769230769232</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
       <c r="E38">
-        <v>0.1353846153846154</v>
+        <v>0.6746153846153846</v>
       </c>
       <c r="F38">
-        <v>0.01153846153846154</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="39" spans="2:6">
       <c r="B39">
-        <v>1.106169296987087</v>
+        <v>0.495</v>
       </c>
       <c r="C39">
-        <v>0.1553846153846154</v>
+        <v>0.004615384615384616</v>
       </c>
       <c r="D39">
         <v>1</v>
       </c>
       <c r="E39">
-        <v>0.1484615384615385</v>
+        <v>0.6792307692307692</v>
       </c>
       <c r="F39">
-        <v>0.01230769230769231</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="40" spans="2:6">
       <c r="B40">
-        <v>1.124118476727785</v>
+        <v>0.2944162436548223</v>
       </c>
       <c r="C40">
-        <v>0.1607692307692308</v>
+        <v>0.004615384615384616</v>
       </c>
       <c r="D40">
         <v>1</v>
       </c>
       <c r="E40">
-        <v>0.1584615384615385</v>
+        <v>0.6792307692307692</v>
       </c>
       <c r="F40">
-        <v>0.01230769230769231</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="41" spans="2:6">
       <c r="B41">
-        <v>1.145027624309392</v>
+        <v>0.1722222222222222</v>
       </c>
       <c r="C41">
-        <v>0.1684615384615385</v>
+        <v>0.005384615384615384</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="E41">
-        <v>0.1669230769230769</v>
+        <v>0.6792307692307692</v>
       </c>
       <c r="F41">
-        <v>0.01307692307692308</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="42" spans="2:6">
       <c r="B42">
-        <v>1.140750670241287</v>
+        <v>0</v>
       </c>
       <c r="C42">
-        <v>0.17</v>
+        <v>0</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E42">
-        <v>0.1807692307692308</v>
+        <v>0</v>
       </c>
       <c r="F42">
-        <v>0.01384615384615385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="2:6">
       <c r="B43">
-        <v>1.138780804150454</v>
+        <v>0</v>
       </c>
       <c r="C43">
-        <v>0.1761538461538462</v>
+        <v>0</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E43">
-        <v>0.1938461538461538</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>0.01461538461538462</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="2:6">
       <c r="B44">
-        <v>1.130489335006273</v>
+        <v>0</v>
       </c>
       <c r="C44">
-        <v>0.1784615384615384</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>0.2061538461538462</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>0.01615384615384615</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="2:6">
       <c r="B45">
-        <v>1.110977080820266</v>
+        <v>0</v>
       </c>
       <c r="C45">
-        <v>0.1838461538461539</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>0.2138461538461539</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>0.01692307692307692</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="2:6">
       <c r="B46">
-        <v>1.09165687426557</v>
+        <v>0</v>
       </c>
       <c r="C46">
-        <v>0.1761538461538462</v>
+        <v>0</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>0.2292307692307692</v>
+        <v>0</v>
       </c>
       <c r="F46">
-        <v>0.02076923076923077</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="2:6">
       <c r="B47">
-        <v>1.061503416856492</v>
+        <v>0</v>
       </c>
       <c r="C47">
-        <v>0.1784615384615384</v>
+        <v>0</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E47">
-        <v>0.2384615384615385</v>
+        <v>0</v>
       </c>
       <c r="F47">
-        <v>0.02076923076923077</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="2:6">
       <c r="B48">
-        <v>1.04661487236404</v>
+        <v>0</v>
       </c>
       <c r="C48">
-        <v>0.1869230769230769</v>
+        <v>0</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E48">
-        <v>0.2453846153846154</v>
+        <v>0</v>
       </c>
       <c r="F48">
-        <v>0.02076923076923077</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="2:6">
       <c r="B49">
-        <v>1.036916395222584</v>
+        <v>0</v>
       </c>
       <c r="C49">
-        <v>0.1930769230769231</v>
+        <v>0</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49">
-        <v>0.2576923076923077</v>
+        <v>0</v>
       </c>
       <c r="F49">
-        <v>0.02076923076923077</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:6">
       <c r="B50">
-        <v>1.053821313240043</v>
+        <v>0</v>
       </c>
       <c r="C50">
-        <v>0.1946153846153846</v>
+        <v>0</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E50">
-        <v>0.2669230769230769</v>
+        <v>0</v>
       </c>
       <c r="F50">
-        <v>0.02384615384615385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="2:6">
       <c r="B51">
-        <v>1.063304721030043</v>
+        <v>0</v>
       </c>
       <c r="C51">
-        <v>0.1876923076923077</v>
+        <v>0</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E51">
-        <v>0.2815384615384615</v>
+        <v>0</v>
       </c>
       <c r="F51">
-        <v>0.02384615384615385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="2:6">
       <c r="B52">
-        <v>1.042417815482503</v>
+        <v>0</v>
       </c>
       <c r="C52">
-        <v>0.1807692307692308</v>
+        <v>0</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E52">
-        <v>0.2938461538461539</v>
+        <v>0</v>
       </c>
       <c r="F52">
-        <v>0.02461538461538462</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="2:6">
       <c r="B53">
-        <v>1.015706806282722</v>
+        <v>0</v>
       </c>
       <c r="C53">
-        <v>0.1830769230769231</v>
+        <v>0</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53">
-        <v>0.3007692307692308</v>
+        <v>0</v>
       </c>
       <c r="F53">
-        <v>0.02538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="2:6">
       <c r="B54">
-        <v>0.9765066394279879</v>
+        <v>0</v>
       </c>
       <c r="C54">
-        <v>0.1838461538461539</v>
+        <v>0</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E54">
-        <v>0.3115384615384615</v>
+        <v>0</v>
       </c>
       <c r="F54">
-        <v>0.02538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="2:6">
       <c r="B55">
-        <v>0.9485368314833502</v>
+        <v>0</v>
       </c>
       <c r="C55">
-        <v>0.1753846153846154</v>
+        <v>0</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E55">
-        <v>0.3238461538461538</v>
+        <v>0</v>
       </c>
       <c r="F55">
-        <v>0.02615384615384615</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="2:6">
       <c r="B56">
-        <v>0.9471007121057985</v>
+        <v>0</v>
       </c>
       <c r="C56">
-        <v>0.1738461538461538</v>
+        <v>0</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56">
-        <v>0.3330769230769231</v>
+        <v>0</v>
       </c>
       <c r="F56">
-        <v>0.02615384615384615</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="2:6">
       <c r="B57">
-        <v>0.9443298969072165</v>
+        <v>0</v>
       </c>
       <c r="C57">
-        <v>0.1715384615384615</v>
+        <v>0</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>0.3415384615384615</v>
+        <v>0</v>
       </c>
       <c r="F57">
-        <v>0.02615384615384615</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="2:6">
       <c r="B58">
-        <v>0.9330543933054393</v>
+        <v>0</v>
       </c>
       <c r="C58">
-        <v>0.1653846153846154</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>0.3546153846153846</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>0.02692307692307692</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="2:6">
       <c r="B59">
-        <v>0.9329787234042553</v>
+        <v>0</v>
       </c>
       <c r="C59">
-        <v>0.1638461538461538</v>
+        <v>0</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E59">
-        <v>0.3630769230769231</v>
+        <v>0</v>
       </c>
       <c r="F59">
-        <v>0.02769230769230769</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:6">
       <c r="B60">
-        <v>0.9226638023630505</v>
+        <v>0</v>
       </c>
       <c r="C60">
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E60">
-        <v>0.3715384615384615</v>
+        <v>0</v>
       </c>
       <c r="F60">
-        <v>0.02846153846153846</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:6">
       <c r="B61">
-        <v>0.9115720524017465</v>
+        <v>0</v>
       </c>
       <c r="C61">
-        <v>0.1530769230769231</v>
+        <v>0</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E61">
-        <v>0.3830769230769231</v>
+        <v>0</v>
       </c>
       <c r="F61">
-        <v>0.02923076923076923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="2:6">
       <c r="B62">
-        <v>0.9035874439461884</v>
+        <v>0</v>
       </c>
       <c r="C62">
-        <v>0.1430769230769231</v>
+        <v>0</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E62">
-        <v>0.3976923076923077</v>
+        <v>0</v>
       </c>
       <c r="F62">
-        <v>0.03</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="2:6">
       <c r="B63">
-        <v>0.8711516533637401</v>
+        <v>0</v>
       </c>
       <c r="C63">
-        <v>0.1315384615384615</v>
+        <v>0</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E63">
-        <v>0.4115384615384615</v>
+        <v>0</v>
       </c>
       <c r="F63">
-        <v>0.03076923076923077</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="2:6">
       <c r="B64">
-        <v>0.8428405122235157</v>
+        <v>0</v>
       </c>
       <c r="C64">
-        <v>0.1292307692307692</v>
+        <v>0</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E64">
-        <v>0.4223076923076923</v>
+        <v>0</v>
       </c>
       <c r="F64">
-        <v>0.03076923076923077</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="2:6">
       <c r="B65">
-        <v>0.8203592814371259</v>
+        <v>0</v>
       </c>
       <c r="C65">
-        <v>0.1230769230769231</v>
+        <v>0</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65">
-        <v>0.43</v>
+        <v>0</v>
       </c>
       <c r="F65">
-        <v>0.03153846153846154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="2:6">
       <c r="B66">
-        <v>0.8089330024813896</v>
+        <v>0</v>
       </c>
       <c r="C66">
-        <v>0.1176923076923077</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E66">
-        <v>0.4376923076923077</v>
+        <v>0</v>
       </c>
       <c r="F66">
-        <v>0.03307692307692308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="2:6">
       <c r="B67">
-        <v>0.8219895287958114</v>
+        <v>0</v>
       </c>
       <c r="C67">
-        <v>0.1130769230769231</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E67">
-        <v>0.4469230769230769</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>0.03307692307692308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="2:6">
       <c r="B68">
-        <v>0.8273480662983425</v>
+        <v>0</v>
       </c>
       <c r="C68">
-        <v>0.1069230769230769</v>
+        <v>0</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E68">
-        <v>0.4538461538461538</v>
+        <v>0</v>
       </c>
       <c r="F68">
-        <v>0.03384615384615385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="2:6">
       <c r="B69">
-        <v>0.8394160583941607</v>
+        <v>0</v>
       </c>
       <c r="C69">
-        <v>0.1046153846153846</v>
+        <v>0</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E69">
-        <v>0.4607692307692308</v>
+        <v>0</v>
       </c>
       <c r="F69">
-        <v>0.03461538461538462</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="2:6">
       <c r="B70">
-        <v>0.8374233128834357</v>
+        <v>0</v>
       </c>
       <c r="C70">
-        <v>0.09538461538461539</v>
+        <v>0</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E70">
-        <v>0.4723076923076923</v>
+        <v>0</v>
       </c>
       <c r="F70">
-        <v>0.03538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="2:6">
       <c r="B71">
-        <v>0.8343949044585988</v>
+        <v>0</v>
       </c>
       <c r="C71">
-        <v>0.09615384615384616</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>0.4769230769230769</v>
+        <v>0</v>
       </c>
       <c r="F71">
-        <v>0.03538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="2:6">
       <c r="B72">
-        <v>0.8414023372287146</v>
+        <v>0</v>
       </c>
       <c r="C72">
-        <v>0.09153846153846154</v>
+        <v>0</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>0.4846153846153846</v>
+        <v>0</v>
       </c>
       <c r="F72">
-        <v>0.03538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="2:6">
       <c r="B73">
-        <v>0.8347826086956521</v>
+        <v>0</v>
       </c>
       <c r="C73">
-        <v>0.08615384615384615</v>
+        <v>0</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E73">
-        <v>0.4907692307692308</v>
+        <v>0</v>
       </c>
       <c r="F73">
-        <v>0.03692307692307693</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="2:6">
       <c r="B74">
-        <v>0.8479853479853479</v>
+        <v>0</v>
       </c>
       <c r="C74">
-        <v>0.0823076923076923</v>
+        <v>0</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74">
-        <v>0.4946153846153846</v>
+        <v>0</v>
       </c>
       <c r="F74">
-        <v>0.03846153846153846</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="2:6">
       <c r="B75">
-        <v>0.8396946564885496</v>
+        <v>0</v>
       </c>
       <c r="C75">
-        <v>0.07846153846153846</v>
+        <v>0</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E75">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F75">
-        <v>0.03923076923076923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="2:6">
       <c r="B76">
-        <v>0.8313492063492063</v>
+        <v>0</v>
       </c>
       <c r="C76">
-        <v>0.07538461538461538</v>
+        <v>0</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E76">
-        <v>0.5053846153846154</v>
+        <v>0</v>
       </c>
       <c r="F76">
-        <v>0.03923076923076923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="2:6">
       <c r="B77">
-        <v>0.8416666666666666</v>
+        <v>0</v>
       </c>
       <c r="C77">
-        <v>0.07461538461538461</v>
+        <v>0</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E77">
-        <v>0.5069230769230769</v>
+        <v>0</v>
       </c>
       <c r="F77">
-        <v>0.03923076923076923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="2:6">
       <c r="B78">
-        <v>0.8488120950323975</v>
+        <v>0</v>
       </c>
       <c r="C78">
-        <v>0.07384615384615385</v>
+        <v>0</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E78">
-        <v>0.5107692307692308</v>
+        <v>0</v>
       </c>
       <c r="F78">
-        <v>0.03923076923076923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="2:6">
       <c r="B79">
-        <v>0.8772727272727273</v>
+        <v>0</v>
       </c>
       <c r="C79">
-        <v>0.07307692307692308</v>
+        <v>0</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E79">
-        <v>0.5138461538461538</v>
+        <v>0</v>
       </c>
       <c r="F79">
-        <v>0.03923076923076923</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="2:6">
       <c r="B80">
-        <v>0.9069212410501193</v>
+        <v>0</v>
       </c>
       <c r="C80">
-        <v>0.07076923076923076</v>
+        <v>0</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E80">
-        <v>0.5169230769230769</v>
+        <v>0</v>
       </c>
       <c r="F80">
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="2:6">
       <c r="B81">
-        <v>0.9158415841584159</v>
+        <v>0</v>
       </c>
       <c r="C81">
-        <v>0.06692307692307692</v>
+        <v>0</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E81">
-        <v>0.5215384615384615</v>
+        <v>0</v>
       </c>
       <c r="F81">
-        <v>0.04</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="2:6">
       <c r="B82">
-        <v>0.9033078880407125</v>
+        <v>0</v>
       </c>
       <c r="C82">
-        <v>0.06230769230769231</v>
+        <v>0</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E82">
-        <v>0.5269230769230769</v>
+        <v>0</v>
       </c>
       <c r="F82">
-        <v>0.04153846153846154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="2:6">
       <c r="B83">
-        <v>0.8678756476683936</v>
+        <v>0</v>
       </c>
       <c r="C83">
-        <v>0.0576923076923077</v>
+        <v>0</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E83">
-        <v>0.5330769230769231</v>
+        <v>0</v>
       </c>
       <c r="F83">
-        <v>0.04153846153846154</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="2:6">
       <c r="B84">
-        <v>0.8263157894736843</v>
+        <v>0</v>
       </c>
       <c r="C84">
-        <v>0.05461538461538461</v>
+        <v>0</v>
       </c>
       <c r="D84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E84">
-        <v>0.5376923076923077</v>
+        <v>0</v>
       </c>
       <c r="F84">
-        <v>0.04230769230769231</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="2:6">
       <c r="B85">
-        <v>0.7864864864864864</v>
+        <v>0</v>
       </c>
       <c r="C85">
-        <v>0.04923076923076923</v>
+        <v>0</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E85">
-        <v>0.5446153846153846</v>
+        <v>0</v>
       </c>
       <c r="F85">
-        <v>0.04230769230769231</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="2:6">
       <c r="B86">
-        <v>0.76056338028169</v>
+        <v>0</v>
       </c>
       <c r="C86">
-        <v>0.04615384615384616</v>
+        <v>0</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E86">
-        <v>0.5476923076923077</v>
+        <v>0</v>
       </c>
       <c r="F86">
-        <v>0.04307692307692308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="2:6">
       <c r="B87">
-        <v>0.7611940298507465</v>
+        <v>0</v>
       </c>
       <c r="C87">
-        <v>0.04615384615384616</v>
+        <v>0</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E87">
-        <v>0.5507692307692308</v>
+        <v>0</v>
       </c>
       <c r="F87">
-        <v>0.04307692307692308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="2:6">
       <c r="B88">
-        <v>0.7770700636942676</v>
+        <v>0</v>
       </c>
       <c r="C88">
-        <v>0.04615384615384616</v>
+        <v>0</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E88">
-        <v>0.5523076923076923</v>
+        <v>0</v>
       </c>
       <c r="F88">
-        <v>0.04307692307692308</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="2:6">
       <c r="B89">
-        <v>0.8316151202749142</v>
+        <v>0</v>
       </c>
       <c r="C89">
-        <v>0.04769230769230769</v>
+        <v>0</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E89">
-        <v>0.5523076923076923</v>
+        <v>0</v>
       </c>
       <c r="F89">
-        <v>0.04384615384615385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="2:6">
       <c r="B90">
-        <v>0.8851851851851853</v>
+        <v>0</v>
       </c>
       <c r="C90">
-        <v>0.04384615384615385</v>
+        <v>0</v>
       </c>
       <c r="D90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E90">
-        <v>0.5576923076923077</v>
+        <v>0</v>
       </c>
       <c r="F90">
-        <v>0.04384615384615385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="2:6">
       <c r="B91">
-        <v>0.9137254901960784</v>
+        <v>0</v>
       </c>
       <c r="C91">
-        <v>0.04153846153846154</v>
+        <v>0</v>
       </c>
       <c r="D91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E91">
-        <v>0.5600000000000001</v>
+        <v>0</v>
       </c>
       <c r="F91">
-        <v>0.04384615384615385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="2:6">
       <c r="B92">
-        <v>0.9262295081967212</v>
+        <v>0</v>
       </c>
       <c r="C92">
-        <v>0.04076923076923077</v>
+        <v>0</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E92">
-        <v>0.5615384615384615</v>
+        <v>0</v>
       </c>
       <c r="F92">
-        <v>0.04384615384615385</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="2:6">
       <c r="B93">
-        <v>0.871900826446281</v>
+        <v>0</v>
       </c>
       <c r="C93">
-        <v>0.03615384615384615</v>
+        <v>0</v>
       </c>
       <c r="D93">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E93">
-        <v>0.566923076923077</v>
+        <v>0</v>
       </c>
       <c r="F93">
-        <v>0.04461538461538461</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="2:6">
       <c r="B94">
-        <v>0.8368200836820083</v>
+        <v>0</v>
       </c>
       <c r="C94">
-        <v>0.03538461538461538</v>
+        <v>0</v>
       </c>
       <c r="D94">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E94">
-        <v>0.5692307692307692</v>
+        <v>0</v>
       </c>
       <c r="F94">
-        <v>0.04461538461538461</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="2:6">
       <c r="B95">
-        <v>0.8068669527896993</v>
+        <v>0</v>
       </c>
       <c r="C95">
-        <v>0.03230769230769231</v>
+        <v>0</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E95">
-        <v>0.5738461538461539</v>
+        <v>0</v>
       </c>
       <c r="F95">
-        <v>0.04461538461538461</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="2:6">
       <c r="B96">
-        <v>0.7831858407079646</v>
+        <v>0</v>
       </c>
       <c r="C96">
-        <v>0.03230769230769231</v>
+        <v>0</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E96">
-        <v>0.5753846153846154</v>
+        <v>0</v>
       </c>
       <c r="F96">
-        <v>0.04461538461538461</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="2:6">
       <c r="B97">
-        <v>0.8056872037914692</v>
+        <v>0</v>
       </c>
       <c r="C97">
-        <v>0.03076923076923077</v>
+        <v>0</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E97">
-        <v>0.5784615384615385</v>
+        <v>0</v>
       </c>
       <c r="F97">
-        <v>0.04461538461538461</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="2:6">
       <c r="B98">
-        <v>0.8100000000000001</v>
+        <v>0</v>
       </c>
       <c r="C98">
-        <v>0.02923076923076923</v>
+        <v>0</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E98">
-        <v>0.5807692307692308</v>
+        <v>0</v>
       </c>
       <c r="F98">
-        <v>0.04461538461538461</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="2:6">
       <c r="B99">
-        <v>0.8085106382978726</v>
+        <v>0</v>
       </c>
       <c r="C99">
-        <v>0.02461538461538462</v>
+        <v>0</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E99">
-        <v>0.5846153846153846</v>
+        <v>0</v>
       </c>
       <c r="F99">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="2:6">
       <c r="B100">
-        <v>0.7740112994350282</v>
+        <v>0</v>
       </c>
       <c r="C100">
-        <v>0.02076923076923077</v>
+        <v>0</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E100">
-        <v>0.5884615384615385</v>
+        <v>0</v>
       </c>
       <c r="F100">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="2:6">
       <c r="B101">
-        <v>0.7176470588235293</v>
+        <v>0</v>
       </c>
       <c r="C101">
-        <v>0.01923076923076923</v>
+        <v>0</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E101">
-        <v>0.59</v>
+        <v>0</v>
       </c>
       <c r="F101">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="2:6">
       <c r="B102">
-        <v>0.6604938271604938</v>
+        <v>0</v>
       </c>
       <c r="C102">
-        <v>0.01769230769230769</v>
+        <v>0</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E102">
-        <v>0.5915384615384616</v>
+        <v>0</v>
       </c>
       <c r="F102">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="2:6">
       <c r="B103">
-        <v>0.6184210526315789</v>
+        <v>0</v>
       </c>
       <c r="C103">
-        <v>0.01461538461538462</v>
+        <v>0</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E103">
-        <v>0.5946153846153847</v>
+        <v>0</v>
       </c>
       <c r="F103">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="2:6">
       <c r="B104">
-        <v>0.6131386861313869</v>
+        <v>0</v>
       </c>
       <c r="C104">
-        <v>0.01307692307692308</v>
+        <v>0</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E104">
-        <v>0.5961538461538461</v>
+        <v>0</v>
       </c>
       <c r="F104">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="2:6">
       <c r="B105">
-        <v>0.6229508196721311</v>
+        <v>0</v>
       </c>
       <c r="C105">
-        <v>0.01307692307692308</v>
+        <v>0</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E105">
-        <v>0.5961538461538461</v>
+        <v>0</v>
       </c>
       <c r="F105">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="2:6">
       <c r="B106">
-        <v>0.6355140186915887</v>
+        <v>0</v>
       </c>
       <c r="C106">
-        <v>0.01153846153846154</v>
+        <v>0</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E106">
-        <v>0.5976923076923077</v>
+        <v>0</v>
       </c>
       <c r="F106">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="2:6">
       <c r="B107">
-        <v>0.6382978723404255</v>
+        <v>0</v>
       </c>
       <c r="C107">
-        <v>0.008461538461538461</v>
+        <v>0</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E107">
-        <v>0.6007692307692307</v>
+        <v>0</v>
       </c>
       <c r="F107">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="2:6">
       <c r="B108">
-        <v>0.6190476190476191</v>
+        <v>0</v>
       </c>
       <c r="C108">
-        <v>0.006923076923076923</v>
+        <v>0</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E108">
-        <v>0.6023076923076923</v>
+        <v>0</v>
       </c>
       <c r="F108">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="2:6">
       <c r="B109">
-        <v>0.5526315789473685</v>
+        <v>0</v>
       </c>
       <c r="C109">
-        <v>0.005384615384615384</v>
+        <v>0</v>
       </c>
       <c r="D109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E109">
-        <v>0.6038461538461538</v>
+        <v>0</v>
       </c>
       <c r="F109">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="2:6">
       <c r="B110">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C110">
-        <v>0.005384615384615384</v>
+        <v>0</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E110">
-        <v>0.6038461538461538</v>
+        <v>0</v>
       </c>
       <c r="F110">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="2:6">
       <c r="B111">
-        <v>0.4833333333333334</v>
+        <v>0</v>
       </c>
       <c r="C111">
-        <v>0.004615384615384616</v>
+        <v>0</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E111">
-        <v>0.6046153846153847</v>
+        <v>0</v>
       </c>
       <c r="F111">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="2:6">
       <c r="B112">
-        <v>0.4807692307692307</v>
+        <v>0</v>
       </c>
       <c r="C112">
-        <v>0.003846153846153846</v>
+        <v>0</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E112">
-        <v>0.6053846153846154</v>
+        <v>0</v>
       </c>
       <c r="F112">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="113" spans="2:6">
       <c r="B113">
-        <v>0.5476190476190476</v>
+        <v>0</v>
       </c>
       <c r="C113">
-        <v>0.003846153846153846</v>
+        <v>0</v>
       </c>
       <c r="D113">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E113">
-        <v>0.6053846153846154</v>
+        <v>0</v>
       </c>
       <c r="F113">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="2:6">
       <c r="B114">
-        <v>0.6176470588235294</v>
+        <v>0</v>
       </c>
       <c r="C114">
-        <v>0.003846153846153846</v>
+        <v>0</v>
       </c>
       <c r="D114">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E114">
-        <v>0.6053846153846154</v>
+        <v>0</v>
       </c>
       <c r="F114">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="2:6">
       <c r="B115">
-        <v>0.689655172413793</v>
+        <v>0</v>
       </c>
       <c r="C115">
-        <v>0.003846153846153846</v>
+        <v>0</v>
       </c>
       <c r="D115">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E115">
-        <v>0.6053846153846154</v>
+        <v>0</v>
       </c>
       <c r="F115">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116" spans="2:6">
       <c r="B116">
-        <v>0.7600000000000001</v>
+        <v>0</v>
       </c>
       <c r="C116">
-        <v>0.003076923076923077</v>
+        <v>0</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E116">
-        <v>0.6061538461538462</v>
+        <v>0</v>
       </c>
       <c r="F116">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117" spans="2:6">
       <c r="B117">
-        <v>0.7826086956521739</v>
+        <v>0</v>
       </c>
       <c r="C117">
-        <v>0.003076923076923077</v>
+        <v>0</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E117">
-        <v>0.6061538461538462</v>
+        <v>0</v>
       </c>
       <c r="F117">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="2:6">
       <c r="B118">
-        <v>0.8095238095238094</v>
+        <v>0</v>
       </c>
       <c r="C118">
-        <v>0.003076923076923077</v>
+        <v>0</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E118">
-        <v>0.6061538461538462</v>
+        <v>0</v>
       </c>
       <c r="F118">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119" spans="2:6">
       <c r="B119">
-        <v>0.7999999999999999</v>
+        <v>0</v>
       </c>
       <c r="C119">
-        <v>0.003076923076923077</v>
+        <v>0</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E119">
-        <v>0.6061538461538462</v>
+        <v>0</v>
       </c>
       <c r="F119">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120" spans="2:6">
       <c r="B120">
-        <v>0.8421052631578947</v>
+        <v>0</v>
       </c>
       <c r="C120">
-        <v>0.003076923076923077</v>
+        <v>0</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E120">
-        <v>0.6061538461538462</v>
+        <v>0</v>
       </c>
       <c r="F120">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="121" spans="2:6">
       <c r="B121">
-        <v>0.8888888888888888</v>
+        <v>0</v>
       </c>
       <c r="C121">
-        <v>0.003076923076923077</v>
+        <v>0</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E121">
-        <v>0.6061538461538462</v>
+        <v>0</v>
       </c>
       <c r="F121">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122" spans="2:6">
       <c r="B122">
-        <v>0.8823529411764707</v>
+        <v>0</v>
       </c>
       <c r="C122">
-        <v>0.002307692307692308</v>
+        <v>0</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E122">
-        <v>0.6069230769230769</v>
+        <v>0</v>
       </c>
       <c r="F122">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="123" spans="2:6">
       <c r="B123">
-        <v>0.8750000000000001</v>
+        <v>0</v>
       </c>
       <c r="C123">
-        <v>0.002307692307692308</v>
+        <v>0</v>
       </c>
       <c r="D123">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E123">
-        <v>0.6069230769230769</v>
+        <v>0</v>
       </c>
       <c r="F123">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="124" spans="2:6">
       <c r="B124">
-        <v>0.8125000000000001</v>
+        <v>0</v>
       </c>
       <c r="C124">
-        <v>0.002307692307692308</v>
+        <v>0</v>
       </c>
       <c r="D124">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E124">
-        <v>0.6069230769230769</v>
+        <v>0</v>
       </c>
       <c r="F124">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="125" spans="2:6">
       <c r="B125">
-        <v>0.7500000000000001</v>
+        <v>0</v>
       </c>
       <c r="C125">
-        <v>0.002307692307692308</v>
+        <v>0</v>
       </c>
       <c r="D125">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E125">
-        <v>0.6069230769230769</v>
+        <v>0</v>
       </c>
       <c r="F125">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126" spans="2:6">
       <c r="B126">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="C126">
-        <v>0.002307692307692308</v>
+        <v>0</v>
       </c>
       <c r="D126">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E126">
-        <v>0.6069230769230769</v>
+        <v>0</v>
       </c>
       <c r="F126">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="127" spans="2:6">
       <c r="B127">
-        <v>0.8571428571428571</v>
+        <v>0</v>
       </c>
       <c r="C127">
-        <v>0.002307692307692308</v>
+        <v>0</v>
       </c>
       <c r="D127">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E127">
-        <v>0.6069230769230769</v>
+        <v>0</v>
       </c>
       <c r="F127">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" spans="2:6">
       <c r="B128">
-        <v>0.8461538461538459</v>
+        <v>0</v>
       </c>
       <c r="C128">
-        <v>0.001538461538461538</v>
+        <v>0</v>
       </c>
       <c r="D128">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E128">
-        <v>0.6076923076923076</v>
+        <v>0</v>
       </c>
       <c r="F128">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="2:6">
       <c r="B129">
-        <v>0.8333333333333333</v>
+        <v>0</v>
       </c>
       <c r="C129">
-        <v>0.001538461538461538</v>
+        <v>0</v>
       </c>
       <c r="D129">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E129">
-        <v>0.6076923076923076</v>
+        <v>0</v>
       </c>
       <c r="F129">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="2:6">
       <c r="B130">
-        <v>0.6666666666666666</v>
+        <v>0</v>
       </c>
       <c r="C130">
-        <v>0.0007692307692307692</v>
+        <v>0</v>
       </c>
       <c r="D130">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E130">
-        <v>0.6084615384615385</v>
+        <v>0</v>
       </c>
       <c r="F130">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="2:6">
       <c r="B131">
-        <v>0.4999999999999999</v>
+        <v>0</v>
       </c>
       <c r="C131">
-        <v>0.0007692307692307692</v>
+        <v>0</v>
       </c>
       <c r="D131">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E131">
-        <v>0.6084615384615385</v>
+        <v>0</v>
       </c>
       <c r="F131">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="2:6">
       <c r="B132">
-        <v>0.4545454545454545</v>
+        <v>0</v>
       </c>
       <c r="C132">
-        <v>0.0007692307692307692</v>
+        <v>0</v>
       </c>
       <c r="D132">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E132">
-        <v>0.6084615384615385</v>
+        <v>0</v>
       </c>
       <c r="F132">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="2:6">
       <c r="B133">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="C133">
-        <v>0.0007692307692307692</v>
+        <v>0</v>
       </c>
       <c r="D133">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E133">
-        <v>0.6084615384615385</v>
+        <v>0</v>
       </c>
       <c r="F133">
-        <v>0.04538461538461538</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="2:6">

</xml_diff>